<commit_message>
mess up dob and start_na also
</commit_message>
<xml_diff>
--- a/data/messy_uc.xlsx
+++ b/data/messy_uc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterhiggins/Documents/RCode/rmedicine-data-cleaning-2023/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pileggis\Documents\gh-personal\rmedicine-data-cleaning-2023\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFB4FD1-A5BC-4246-A283-935F70A86EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30855879-F140-48B5-81ED-D5ED64A04739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21600" windowHeight="37900" activeTab="2" xr2:uid="{C3B41A98-E045-B641-B5DC-D433CA053FBE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{C3B41A98-E045-B641-B5DC-D433CA053FBE}"/>
   </bookViews>
   <sheets>
     <sheet name="Explainer" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="364">
   <si>
     <t>Your well-meaning research assistant/med student has extracted data from the medical record into Excel</t>
   </si>
@@ -1093,6 +1093,42 @@
   </si>
   <si>
     <t>291K/microL</t>
+  </si>
+  <si>
+    <t>137mmol/L</t>
+  </si>
+  <si>
+    <t>142mmol/L</t>
+  </si>
+  <si>
+    <t>140mmol/L</t>
+  </si>
+  <si>
+    <t>139mmol/L</t>
+  </si>
+  <si>
+    <t>144mmol/L</t>
+  </si>
+  <si>
+    <t>145mmol/L</t>
+  </si>
+  <si>
+    <t>138mmol/L</t>
+  </si>
+  <si>
+    <t>143mmol/L</t>
+  </si>
+  <si>
+    <t>136mmol/L</t>
+  </si>
+  <si>
+    <t>135mmol/L</t>
+  </si>
+  <si>
+    <t>141mmol/L</t>
+  </si>
+  <si>
+    <t>133mmol/L</t>
   </si>
 </sst>
 </file>
@@ -1102,7 +1138,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1184,7 +1220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1198,6 +1234,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1518,29 +1555,29 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>314</v>
       </c>
@@ -1555,16 +1592,16 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="17.83203125" customWidth="1"/>
     <col min="2" max="2" width="43.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -1578,7 +1615,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1592,7 +1629,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1603,7 +1640,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1617,7 +1654,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1628,7 +1665,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1639,7 +1676,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1653,7 +1690,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1667,7 +1704,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1681,7 +1718,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1695,7 +1732,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1712,7 +1749,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1729,7 +1766,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1746,7 +1783,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1763,7 +1800,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1780,7 +1817,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1797,7 +1834,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1811,7 +1848,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1825,7 +1862,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1839,7 +1876,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1853,7 +1890,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1867,7 +1904,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1881,7 +1918,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1895,7 +1932,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1909,7 +1946,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -1926,7 +1963,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1943,7 +1980,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1960,7 +1997,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1977,7 +2014,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -1994,7 +2031,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -2011,7 +2048,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -2025,7 +2062,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -2039,7 +2076,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -2053,7 +2090,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -2077,11 +2114,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2E3CCE-D9A6-4043-B4E6-790885873B0A}">
   <dimension ref="A1:AL38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
+      <selection activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="5" max="5" width="18.5" customWidth="1"/>
     <col min="16" max="16" width="11.6640625" bestFit="1" customWidth="1"/>
@@ -2091,22 +2128,22 @@
     <col min="37" max="37" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:38">
       <c r="A1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:38">
       <c r="A2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:38">
       <c r="A3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:38">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -2219,7 +2256,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:38">
       <c r="A8" s="3" t="s">
         <v>95</v>
       </c>
@@ -2235,7 +2272,7 @@
       <c r="E8" t="s">
         <v>278</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="13">
         <v>38359</v>
       </c>
       <c r="G8" s="4"/>
@@ -2250,27 +2287,27 @@
       </c>
       <c r="K8" s="8">
         <f ca="1">J8*25 + 5* RAND()</f>
-        <v>76.752328986670321</v>
+        <v>77.395707089687207</v>
       </c>
       <c r="L8" s="8">
         <f ca="1">J8* 25 + 6* RAND()</f>
-        <v>75.961387131445022</v>
+        <v>75.571492959177732</v>
       </c>
       <c r="M8" s="8">
         <f ca="1" xml:space="preserve"> J8*26 + 5 * RAND()</f>
-        <v>80.97914593817346</v>
+        <v>78.785710925765727</v>
       </c>
       <c r="N8" s="8">
         <f ca="1" xml:space="preserve"> J8 *14 + 10* RAND()</f>
-        <v>45.790671182036412</v>
+        <v>49.664470834109785</v>
       </c>
       <c r="O8" s="8">
         <f ca="1" xml:space="preserve"> J8 *22 + 15* RAND()</f>
-        <v>76.532259264609223</v>
+        <v>76.862692656240355</v>
       </c>
       <c r="P8" s="8">
         <f ca="1">J8 * 28 + 4* RAND()</f>
-        <v>85.637667382876018</v>
+        <v>87.037412004128825</v>
       </c>
       <c r="Q8">
         <v>8.1999999999999993</v>
@@ -2278,8 +2315,8 @@
       <c r="R8" t="s">
         <v>325</v>
       </c>
-      <c r="S8">
-        <v>137</v>
+      <c r="S8" t="s">
+        <v>352</v>
       </c>
       <c r="T8">
         <v>3.7</v>
@@ -2298,42 +2335,42 @@
       </c>
       <c r="Y8" s="8">
         <f ca="1" xml:space="preserve"> K8-22*(J8-X8)</f>
-        <v>10.752328986670321</v>
+        <v>11.395707089687207</v>
       </c>
       <c r="Z8" s="8">
         <f ca="1" xml:space="preserve"> L8-20*(J8-X8)</f>
-        <v>15.961387131445022</v>
+        <v>15.571492959177732</v>
       </c>
       <c r="AA8" s="8">
         <f ca="1" xml:space="preserve"> M8-24*(J8-X8)</f>
-        <v>8.9791459381734597</v>
+        <v>6.7857109257657271</v>
       </c>
       <c r="AB8" s="8">
         <f ca="1" xml:space="preserve"> N8-9*(J8-X8)</f>
-        <v>18.790671182036412</v>
+        <v>22.664470834109785</v>
       </c>
       <c r="AC8" s="8">
         <f ca="1" xml:space="preserve"> O8-14*(J8-X8)+ 6*RAND()</f>
-        <v>37.599311111322251</v>
+        <v>38.794885130798008</v>
       </c>
       <c r="AD8" s="8">
         <f ca="1" xml:space="preserve"> P8-27*(J8-X8)+ 3*RAND()</f>
-        <v>6.1602411976853428</v>
+        <v>7.7243079127115006</v>
       </c>
       <c r="AE8" s="7">
         <f ca="1">IF(B8 ="upa", Q8 +1.5* RAND()*0.8, Q8 +1.5* RAND())</f>
-        <v>8.7671052376987539</v>
+        <v>8.5991867886566062</v>
       </c>
       <c r="AF8" s="8">
         <v>201</v>
       </c>
-      <c r="AG8" s="8">
+      <c r="AG8" s="8" t="e">
         <f ca="1" xml:space="preserve"> S8 + 0.5* RAND()</f>
-        <v>137.43980106296667</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AH8" s="7">
         <f ca="1">T8 + 0.3* RAND()</f>
-        <v>3.7533806366658795</v>
+        <v>3.8442296870166284</v>
       </c>
       <c r="AI8" s="5" t="s">
         <v>192</v>
@@ -2348,7 +2385,7 @@
         <v>96074</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:38">
       <c r="A9" s="3" t="s">
         <v>96</v>
       </c>
@@ -2364,7 +2401,7 @@
       <c r="E9" t="s">
         <v>278</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="13">
         <v>13618</v>
       </c>
       <c r="G9" s="4"/>
@@ -2379,27 +2416,27 @@
       </c>
       <c r="K9" s="8">
         <f t="shared" ref="K9:K38" ca="1" si="0">J9*25 + 5* RAND()</f>
-        <v>54.762925600617621</v>
+        <v>52.473553638474939</v>
       </c>
       <c r="L9" s="8">
         <f t="shared" ref="L9:L38" ca="1" si="1">J9* 25 + 6* RAND()</f>
-        <v>53.903638025524103</v>
+        <v>54.111212500317251</v>
       </c>
       <c r="M9" s="8">
         <f t="shared" ref="M9:M38" ca="1" si="2" xml:space="preserve"> J9*26 + 5 * RAND()</f>
-        <v>52.620294148474223</v>
+        <v>53.429761211289502</v>
       </c>
       <c r="N9" s="8">
         <f t="shared" ref="N9:N38" ca="1" si="3" xml:space="preserve"> J9 *14 + 10* RAND()</f>
-        <v>29.52532422974468</v>
+        <v>30.954408451998606</v>
       </c>
       <c r="O9" s="8">
         <f t="shared" ref="O9:O38" ca="1" si="4" xml:space="preserve"> J9 *22 + 15* RAND()</f>
-        <v>47.20611985487006</v>
+        <v>50.728991566923426</v>
       </c>
       <c r="P9" s="8">
         <f t="shared" ref="P9:P38" ca="1" si="5">J9 * 28 + 4* RAND()</f>
-        <v>56.786930044864469</v>
+        <v>56.573732071317323</v>
       </c>
       <c r="Q9">
         <v>10.1</v>
@@ -2407,8 +2444,8 @@
       <c r="R9" t="s">
         <v>326</v>
       </c>
-      <c r="S9">
-        <v>142</v>
+      <c r="S9" t="s">
+        <v>353</v>
       </c>
       <c r="T9">
         <v>4.0999999999999996</v>
@@ -2427,42 +2464,42 @@
       </c>
       <c r="Y9" s="8">
         <f t="shared" ref="Y9:Y38" ca="1" si="6" xml:space="preserve"> K9-22*(J9-X9)</f>
-        <v>32.762925600617621</v>
+        <v>30.473553638474939</v>
       </c>
       <c r="Z9" s="8">
         <f t="shared" ref="Z9:Z38" ca="1" si="7" xml:space="preserve"> L9-20*(J9-X9)</f>
-        <v>33.903638025524103</v>
+        <v>34.111212500317251</v>
       </c>
       <c r="AA9" s="8">
         <f t="shared" ref="AA9:AA38" ca="1" si="8" xml:space="preserve"> M9-24*(J9-X9)</f>
-        <v>28.620294148474223</v>
+        <v>29.429761211289502</v>
       </c>
       <c r="AB9" s="8">
         <f t="shared" ref="AB9:AB38" ca="1" si="9" xml:space="preserve"> N9-9*(J9-X9)</f>
-        <v>20.52532422974468</v>
+        <v>21.954408451998606</v>
       </c>
       <c r="AC9" s="8">
         <f t="shared" ref="AC9:AC38" ca="1" si="10" xml:space="preserve"> O9-14*(J9-X9)+ 6*RAND()</f>
-        <v>38.351769832070474</v>
+        <v>37.015601200697233</v>
       </c>
       <c r="AD9" s="8">
         <f t="shared" ref="AD9:AD38" ca="1" si="11" xml:space="preserve"> P9-27*(J9-X9)+ 3*RAND()</f>
-        <v>30.431701710090419</v>
+        <v>31.372902794518804</v>
       </c>
       <c r="AE9" s="7">
         <f t="shared" ref="AE9:AE38" ca="1" si="12">IF(B9 ="upa", Q9 +1.5* RAND()*0.8, Q9 +1.5* RAND())</f>
-        <v>10.821687316157517</v>
+        <v>10.644691386643276</v>
       </c>
       <c r="AF9" s="8">
         <v>340</v>
       </c>
-      <c r="AG9" s="8">
+      <c r="AG9" s="8" t="e">
         <f t="shared" ref="AG9:AG38" ca="1" si="13" xml:space="preserve"> S9 + 0.5* RAND()</f>
-        <v>142.23751803540637</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AH9" s="7">
         <f t="shared" ref="AH9:AH38" ca="1" si="14">T9 + 0.3* RAND()</f>
-        <v>4.3380459653250707</v>
+        <v>4.1756809188999311</v>
       </c>
       <c r="AI9" s="5" t="s">
         <v>195</v>
@@ -2477,7 +2514,7 @@
         <v>11264</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:38">
       <c r="A10" s="3" t="s">
         <v>97</v>
       </c>
@@ -2493,7 +2530,7 @@
       <c r="E10" t="s">
         <v>279</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="13">
         <v>16959</v>
       </c>
       <c r="G10" s="4"/>
@@ -2508,27 +2545,27 @@
       </c>
       <c r="K10" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>26.479559943757469</v>
+        <v>28.518112793694499</v>
       </c>
       <c r="L10" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>25.47453411493785</v>
+        <v>27.053633265569317</v>
       </c>
       <c r="M10" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>26.397374773112755</v>
+        <v>30.577025838545786</v>
       </c>
       <c r="N10" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>18.605420774580466</v>
+        <v>14.44579435445258</v>
       </c>
       <c r="O10" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>36.191034166917191</v>
+        <v>28.793691111661211</v>
       </c>
       <c r="P10" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>30.409435853509514</v>
+        <v>31.877770585570026</v>
       </c>
       <c r="Q10">
         <v>5.5</v>
@@ -2536,8 +2573,8 @@
       <c r="R10" t="s">
         <v>327</v>
       </c>
-      <c r="S10">
-        <v>140</v>
+      <c r="S10" t="s">
+        <v>354</v>
       </c>
       <c r="T10">
         <v>4.3</v>
@@ -2556,27 +2593,27 @@
       </c>
       <c r="Y10" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>26.479559943757469</v>
+        <v>28.518112793694499</v>
       </c>
       <c r="Z10" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>25.47453411493785</v>
+        <v>27.053633265569317</v>
       </c>
       <c r="AA10" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>26.397374773112755</v>
+        <v>30.577025838545786</v>
       </c>
       <c r="AB10" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>18.605420774580466</v>
+        <v>14.44579435445258</v>
       </c>
       <c r="AC10" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>38.554916491393953</v>
+        <v>29.336190842822745</v>
       </c>
       <c r="AD10" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>33.268545815948379</v>
+        <v>33.563118436128839</v>
       </c>
       <c r="AE10" s="7">
         <v>3</v>
@@ -2584,13 +2621,13 @@
       <c r="AF10" s="8">
         <v>256</v>
       </c>
-      <c r="AG10" s="8">
+      <c r="AG10" s="8" t="e">
         <f t="shared" ca="1" si="13"/>
-        <v>140.00957054908491</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AH10" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>4.4821475388048215</v>
+        <v>4.4319755120434223</v>
       </c>
       <c r="AI10" s="5" t="s">
         <v>198</v>
@@ -2605,7 +2642,7 @@
         <v>57246</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:38">
       <c r="A11" s="3" t="s">
         <v>98</v>
       </c>
@@ -2621,7 +2658,7 @@
       <c r="E11" t="s">
         <v>278</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="13">
         <v>23206</v>
       </c>
       <c r="G11" s="4"/>
@@ -2636,27 +2673,27 @@
       </c>
       <c r="K11" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>76.33435626377269</v>
+        <v>76.58245982952684</v>
       </c>
       <c r="L11" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>80.304923796567081</v>
+        <v>79.335195839389684</v>
       </c>
       <c r="M11" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>79.176762566079887</v>
+        <v>80.886180167947145</v>
       </c>
       <c r="N11" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>48.792379512010363</v>
+        <v>51.835917542399272</v>
       </c>
       <c r="O11" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>75.083923111333803</v>
+        <v>80.181408383227534</v>
       </c>
       <c r="P11" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>86.307327572414763</v>
+        <v>86.034990715329002</v>
       </c>
       <c r="Q11">
         <v>4.7</v>
@@ -2664,8 +2701,8 @@
       <c r="R11" t="s">
         <v>328</v>
       </c>
-      <c r="S11">
-        <v>139</v>
+      <c r="S11" t="s">
+        <v>355</v>
       </c>
       <c r="T11">
         <v>3.5</v>
@@ -2684,42 +2721,42 @@
       </c>
       <c r="Y11" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>32.33435626377269</v>
+        <v>32.58245982952684</v>
       </c>
       <c r="Z11" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>40.304923796567081</v>
+        <v>39.335195839389684</v>
       </c>
       <c r="AA11" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>31.176762566079887</v>
+        <v>32.886180167947145</v>
       </c>
       <c r="AB11" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>30.792379512010363</v>
+        <v>33.835917542399272</v>
       </c>
       <c r="AC11" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>50.160241148711833</v>
+        <v>55.964249090294992</v>
       </c>
       <c r="AD11" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>33.862267398987846</v>
+        <v>34.716601709177581</v>
       </c>
       <c r="AE11" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>5.1386650393489894</v>
+        <v>5.027880204555518</v>
       </c>
       <c r="AF11" s="8">
         <v>327</v>
       </c>
-      <c r="AG11" s="8">
+      <c r="AG11" s="8" t="e">
         <f t="shared" ca="1" si="13"/>
-        <v>139.14752070056286</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AH11" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>3.5040682130225389</v>
+        <v>3.5350948530846789</v>
       </c>
       <c r="AI11" s="5" t="s">
         <v>201</v>
@@ -2734,7 +2771,7 @@
         <v>31457</v>
       </c>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:38">
       <c r="A12" s="3" t="s">
         <v>99</v>
       </c>
@@ -2750,7 +2787,7 @@
       <c r="E12" t="s">
         <v>280</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="13">
         <v>28622</v>
       </c>
       <c r="G12" s="4"/>
@@ -2765,27 +2802,27 @@
       </c>
       <c r="K12" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>76.201826265523522</v>
+        <v>77.078132301936236</v>
       </c>
       <c r="L12" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>77.265562256130721</v>
+        <v>77.859580986363056</v>
       </c>
       <c r="M12" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>81.726397083921825</v>
+        <v>80.028365990704103</v>
       </c>
       <c r="N12" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>45.825449543824028</v>
+        <v>43.948922633756297</v>
       </c>
       <c r="O12" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>73.918506323771823</v>
+        <v>71.759208903120197</v>
       </c>
       <c r="P12" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>84.211479372061589</v>
+        <v>87.758663510865873</v>
       </c>
       <c r="Q12">
         <v>8.9</v>
@@ -2793,8 +2830,8 @@
       <c r="R12" t="s">
         <v>329</v>
       </c>
-      <c r="S12">
-        <v>144</v>
+      <c r="S12" t="s">
+        <v>356</v>
       </c>
       <c r="T12">
         <v>4</v>
@@ -2813,27 +2850,27 @@
       </c>
       <c r="Y12" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>54.201826265523522</v>
+        <v>55.078132301936236</v>
       </c>
       <c r="Z12" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>57.265562256130721</v>
+        <v>57.859580986363056</v>
       </c>
       <c r="AA12" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>57.726397083921825</v>
+        <v>56.028365990704103</v>
       </c>
       <c r="AB12" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>36.825449543824028</v>
+        <v>34.948922633756297</v>
       </c>
       <c r="AC12" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>65.571325347787607</v>
+        <v>63.018882114525852</v>
       </c>
       <c r="AD12" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>60.187569452971935</v>
+        <v>61.633098344746031</v>
       </c>
       <c r="AE12" s="7">
         <v>4.8</v>
@@ -2841,13 +2878,13 @@
       <c r="AF12" s="8">
         <v>432</v>
       </c>
-      <c r="AG12" s="8">
+      <c r="AG12" s="8" t="e">
         <f t="shared" ca="1" si="13"/>
-        <v>144.13269799242084</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AH12" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>4.2626127190982617</v>
+        <v>4.0714819133176592</v>
       </c>
       <c r="AI12" s="5" t="s">
         <v>204</v>
@@ -2862,7 +2899,7 @@
         <v>30711</v>
       </c>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:38">
       <c r="A13" s="3" t="s">
         <v>100</v>
       </c>
@@ -2878,7 +2915,7 @@
       <c r="E13" t="s">
         <v>281</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="13">
         <v>33697</v>
       </c>
       <c r="G13" s="4"/>
@@ -2893,27 +2930,27 @@
       </c>
       <c r="K13" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>50.201036351485854</v>
+        <v>52.690537179484288</v>
       </c>
       <c r="L13" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>55.146478680361916</v>
+        <v>53.932627568006758</v>
       </c>
       <c r="M13" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>54.551465467363457</v>
+        <v>54.306973375632992</v>
       </c>
       <c r="N13" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>31.31784007441626</v>
+        <v>32.735726709985457</v>
       </c>
       <c r="O13" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>45.616137810750438</v>
+        <v>46.837736076125836</v>
       </c>
       <c r="P13" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>56.225867158749665</v>
+        <v>56.276592489518407</v>
       </c>
       <c r="Q13">
         <v>9.3000000000000007</v>
@@ -2921,8 +2958,8 @@
       <c r="R13" t="s">
         <v>330</v>
       </c>
-      <c r="S13">
-        <v>145</v>
+      <c r="S13" t="s">
+        <v>357</v>
       </c>
       <c r="T13">
         <v>4.4000000000000004</v>
@@ -2941,42 +2978,42 @@
       </c>
       <c r="Y13" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>28.201036351485854</v>
+        <v>30.690537179484288</v>
       </c>
       <c r="Z13" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>35.146478680361916</v>
+        <v>33.932627568006758</v>
       </c>
       <c r="AA13" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>30.551465467363457</v>
+        <v>30.306973375632992</v>
       </c>
       <c r="AB13" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>22.31784007441626</v>
+        <v>23.735726709985457</v>
       </c>
       <c r="AC13" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>33.451032786628161</v>
+        <v>35.823768389183492</v>
       </c>
       <c r="AD13" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>31.700368580893883</v>
+        <v>29.834076609592881</v>
       </c>
       <c r="AE13" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>9.5332694045400874</v>
+        <v>9.8411770687840185</v>
       </c>
       <c r="AF13" s="8">
         <v>348</v>
       </c>
-      <c r="AG13" s="8">
+      <c r="AG13" s="8" t="e">
         <f t="shared" ca="1" si="13"/>
-        <v>145.32933746710265</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AH13" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>4.6946160666024088</v>
+        <v>4.4564715399867412</v>
       </c>
       <c r="AI13" s="5" t="s">
         <v>207</v>
@@ -2991,7 +3028,7 @@
         <v>52722</v>
       </c>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:38">
       <c r="A14" s="3" t="s">
         <v>101</v>
       </c>
@@ -3007,7 +3044,7 @@
       <c r="E14" t="s">
         <v>282</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="13">
         <v>20323</v>
       </c>
       <c r="G14" s="4"/>
@@ -3022,27 +3059,27 @@
       </c>
       <c r="K14" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>76.701273930144666</v>
+        <v>78.029635813522603</v>
       </c>
       <c r="L14" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>78.368093986396872</v>
+        <v>80.314666841608073</v>
       </c>
       <c r="M14" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>80.362641516420965</v>
+        <v>80.405874884577472</v>
       </c>
       <c r="N14" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>51.212073437893828</v>
+        <v>44.450003619478046</v>
       </c>
       <c r="O14" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>77.182832476155411</v>
+        <v>72.174223680967174</v>
       </c>
       <c r="P14" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>85.743591046271831</v>
+        <v>84.869574929335613</v>
       </c>
       <c r="Q14">
         <v>5.6</v>
@@ -3050,8 +3087,8 @@
       <c r="R14" t="s">
         <v>331</v>
       </c>
-      <c r="S14">
-        <v>142</v>
+      <c r="S14" t="s">
+        <v>353</v>
       </c>
       <c r="T14">
         <v>3.6</v>
@@ -3070,42 +3107,42 @@
       </c>
       <c r="Y14" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>54.701273930144666</v>
+        <v>56.029635813522603</v>
       </c>
       <c r="Z14" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>58.368093986396872</v>
+        <v>60.314666841608073</v>
       </c>
       <c r="AA14" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>56.362641516420965</v>
+        <v>56.405874884577472</v>
       </c>
       <c r="AB14" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>42.212073437893828</v>
+        <v>35.450003619478046</v>
       </c>
       <c r="AC14" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>63.50933803159878</v>
+        <v>59.187143457162918</v>
       </c>
       <c r="AD14" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>59.180444091647736</v>
+        <v>60.272050880074822</v>
       </c>
       <c r="AE14" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>6.0341342837436809</v>
+        <v>5.8698426976681954</v>
       </c>
       <c r="AF14" s="8">
         <v>181</v>
       </c>
-      <c r="AG14" s="8">
+      <c r="AG14" s="8" t="e">
         <f t="shared" ca="1" si="13"/>
-        <v>142.01376899958834</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AH14" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>3.629701816692442</v>
+        <v>3.8040083057831025</v>
       </c>
       <c r="AI14" s="5" t="s">
         <v>210</v>
@@ -3120,7 +3157,7 @@
         <v>48086</v>
       </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:38">
       <c r="A15" s="3" t="s">
         <v>102</v>
       </c>
@@ -3136,7 +3173,7 @@
       <c r="E15" t="s">
         <v>283</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="13">
         <v>27283</v>
       </c>
       <c r="G15" s="4"/>
@@ -3151,27 +3188,27 @@
       </c>
       <c r="K15" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>75.251428421064062</v>
+        <v>79.417740689710314</v>
       </c>
       <c r="L15" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>79.140209916358344</v>
+        <v>78.162622240437145</v>
       </c>
       <c r="M15" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>80.569714506311627</v>
+        <v>82.619855221663997</v>
       </c>
       <c r="N15" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>48.569867314318543</v>
+        <v>45.343555656816527</v>
       </c>
       <c r="O15" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>72.441742468974098</v>
+        <v>80.961274998260961</v>
       </c>
       <c r="P15" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>86.543075444180602</v>
+        <v>84.815926763435428</v>
       </c>
       <c r="Q15">
         <v>9.6999999999999993</v>
@@ -3179,8 +3216,8 @@
       <c r="R15" t="s">
         <v>332</v>
       </c>
-      <c r="S15">
-        <v>138</v>
+      <c r="S15" t="s">
+        <v>358</v>
       </c>
       <c r="T15">
         <v>4.5</v>
@@ -3199,27 +3236,27 @@
       </c>
       <c r="Y15" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>53.251428421064062</v>
+        <v>57.417740689710314</v>
       </c>
       <c r="Z15" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>59.140209916358344</v>
+        <v>58.162622240437145</v>
       </c>
       <c r="AA15" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>56.569714506311627</v>
+        <v>58.619855221663997</v>
       </c>
       <c r="AB15" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>39.569867314318543</v>
+        <v>36.343555656816527</v>
       </c>
       <c r="AC15" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>64.343989541290298</v>
+        <v>70.871157842071199</v>
       </c>
       <c r="AD15" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>60.957083871659869</v>
+        <v>59.517726400153428</v>
       </c>
       <c r="AE15" s="7">
         <v>4.9000000000000004</v>
@@ -3227,13 +3264,13 @@
       <c r="AF15" s="8">
         <v>128</v>
       </c>
-      <c r="AG15" s="8">
+      <c r="AG15" s="8" t="e">
         <f t="shared" ca="1" si="13"/>
-        <v>138.23491951601642</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AH15" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>4.6118698504400193</v>
+        <v>4.6028187814314716</v>
       </c>
       <c r="AI15" s="5" t="s">
         <v>213</v>
@@ -3248,7 +3285,7 @@
         <v>50784</v>
       </c>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:38">
       <c r="A16" s="3" t="s">
         <v>103</v>
       </c>
@@ -3264,7 +3301,7 @@
       <c r="E16" t="s">
         <v>278</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="13">
         <v>31000</v>
       </c>
       <c r="G16" s="4"/>
@@ -3279,27 +3316,27 @@
       </c>
       <c r="K16" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>52.064572744454544</v>
+        <v>50.457859258444074</v>
       </c>
       <c r="L16" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>52.129639996653651</v>
+        <v>52.033617489181125</v>
       </c>
       <c r="M16" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>54.149332505731657</v>
+        <v>54.081207277683689</v>
       </c>
       <c r="N16" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>30.186469874977586</v>
+        <v>37.112809023392508</v>
       </c>
       <c r="O16" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>48.471640834105266</v>
+        <v>57.504151885146584</v>
       </c>
       <c r="P16" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>58.908259742791273</v>
+        <v>57.684203244764717</v>
       </c>
       <c r="Q16">
         <v>8.3000000000000007</v>
@@ -3307,8 +3344,8 @@
       <c r="R16" t="s">
         <v>333</v>
       </c>
-      <c r="S16">
-        <v>140</v>
+      <c r="S16" t="s">
+        <v>354</v>
       </c>
       <c r="T16">
         <v>4.3</v>
@@ -3327,42 +3364,42 @@
       </c>
       <c r="Y16" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>8.0645727444545443</v>
+        <v>6.4578592584440742</v>
       </c>
       <c r="Z16" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>12.129639996653651</v>
+        <v>12.033617489181125</v>
       </c>
       <c r="AA16" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>6.1493325057316568</v>
+        <v>6.0812072776836885</v>
       </c>
       <c r="AB16" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>12.186469874977586</v>
+        <v>19.112809023392508</v>
       </c>
       <c r="AC16" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>21.208889417377435</v>
+        <v>35.271862195951869</v>
       </c>
       <c r="AD16" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>7.2845156988204316</v>
+        <v>6.4408767835455043</v>
       </c>
       <c r="AE16" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>8.7394902107286754</v>
+        <v>9.3186188309606344</v>
       </c>
       <c r="AF16" s="8">
         <v>135</v>
       </c>
-      <c r="AG16" s="8">
+      <c r="AG16" s="8" t="e">
         <f t="shared" ca="1" si="13"/>
-        <v>140.31406046503048</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AH16" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>4.4363886153842031</v>
+        <v>4.4311454099701493</v>
       </c>
       <c r="AI16" s="5" t="s">
         <v>215</v>
@@ -3377,7 +3414,7 @@
         <v>64711</v>
       </c>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:38">
       <c r="A17" s="3" t="s">
         <v>104</v>
       </c>
@@ -3393,7 +3430,7 @@
       <c r="E17" t="s">
         <v>278</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="13">
         <v>26653</v>
       </c>
       <c r="G17" s="4"/>
@@ -3408,27 +3445,27 @@
       </c>
       <c r="K17" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>79.839036589894107</v>
+        <v>77.374157230637337</v>
       </c>
       <c r="L17" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>75.61796262879848</v>
+        <v>79.766075332759044</v>
       </c>
       <c r="M17" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>78.859450504972301</v>
+        <v>79.074002813637364</v>
       </c>
       <c r="N17" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>49.63826459047079</v>
+        <v>51.10591397561268</v>
       </c>
       <c r="O17" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>75.615707003612243</v>
+        <v>78.540319612546881</v>
       </c>
       <c r="P17" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>86.583339511161171</v>
+        <v>86.051557487358778</v>
       </c>
       <c r="Q17">
         <v>7.6</v>
@@ -3436,8 +3473,8 @@
       <c r="R17" t="s">
         <v>334</v>
       </c>
-      <c r="S17">
-        <v>137</v>
+      <c r="S17" t="s">
+        <v>352</v>
       </c>
       <c r="T17">
         <v>3.8</v>
@@ -3456,27 +3493,27 @@
       </c>
       <c r="Y17" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>35.839036589894107</v>
+        <v>33.374157230637337</v>
       </c>
       <c r="Z17" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>35.61796262879848</v>
+        <v>39.766075332759044</v>
       </c>
       <c r="AA17" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>30.859450504972301</v>
+        <v>31.074002813637364</v>
       </c>
       <c r="AB17" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>31.63826459047079</v>
+        <v>33.10591397561268</v>
       </c>
       <c r="AC17" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>50.679174853088178</v>
+        <v>54.196357092228794</v>
       </c>
       <c r="AD17" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>33.249219969514364</v>
+        <v>33.288576296959846</v>
       </c>
       <c r="AE17" s="7">
         <v>4.4000000000000004</v>
@@ -3484,13 +3521,13 @@
       <c r="AF17" s="8">
         <v>238</v>
       </c>
-      <c r="AG17" s="8">
+      <c r="AG17" s="8" t="e">
         <f t="shared" ca="1" si="13"/>
-        <v>137.48222587393226</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AH17" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>3.9206680572158183</v>
+        <v>3.8766705236733965</v>
       </c>
       <c r="AI17" s="5" t="s">
         <v>218</v>
@@ -3505,7 +3542,7 @@
         <v>33707</v>
       </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:38">
       <c r="A18" s="3" t="s">
         <v>105</v>
       </c>
@@ -3521,7 +3558,7 @@
       <c r="E18" t="s">
         <v>284</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="13">
         <v>34617</v>
       </c>
       <c r="G18" s="4"/>
@@ -3536,27 +3573,27 @@
       </c>
       <c r="K18" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>75.453988573810491</v>
+        <v>77.447421245422476</v>
       </c>
       <c r="L18" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>80.112600578253151</v>
+        <v>76.098985004396113</v>
       </c>
       <c r="M18" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>81.25259624686187</v>
+        <v>78.770126928081197</v>
       </c>
       <c r="N18" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>42.983336498422481</v>
+        <v>44.676959457398759</v>
       </c>
       <c r="O18" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>68.570627856325629</v>
+        <v>71.055717729270583</v>
       </c>
       <c r="P18" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>86.91993860546836</v>
+        <v>85.214116555222731</v>
       </c>
       <c r="Q18">
         <v>9.1999999999999993</v>
@@ -3564,8 +3601,8 @@
       <c r="R18" t="s">
         <v>335</v>
       </c>
-      <c r="S18">
-        <v>143</v>
+      <c r="S18" t="s">
+        <v>359</v>
       </c>
       <c r="T18">
         <v>3.6</v>
@@ -3584,42 +3621,42 @@
       </c>
       <c r="Y18" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>9.4539885738104914</v>
+        <v>11.447421245422476</v>
       </c>
       <c r="Z18" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>20.112600578253151</v>
+        <v>16.098985004396113</v>
       </c>
       <c r="AA18" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>9.2525962468618701</v>
+        <v>6.7701269280811971</v>
       </c>
       <c r="AB18" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>15.983336498422481</v>
+        <v>17.676959457398759</v>
       </c>
       <c r="AC18" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>28.368324421986486</v>
+        <v>32.034063339102154</v>
       </c>
       <c r="AD18" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>8.6845565503631565</v>
+        <v>6.9605647288648838</v>
       </c>
       <c r="AE18" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>10.374726887470887</v>
+        <v>10.017911529361267</v>
       </c>
       <c r="AF18" s="8">
         <v>288</v>
       </c>
-      <c r="AG18" s="8">
+      <c r="AG18" s="8" t="e">
         <f t="shared" ca="1" si="13"/>
-        <v>143.08852667082749</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AH18" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>3.8769300049727464</v>
+        <v>3.6103003129935454</v>
       </c>
       <c r="AI18" s="5" t="s">
         <v>221</v>
@@ -3634,7 +3671,7 @@
         <v>69601</v>
       </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:38">
       <c r="A19" s="3" t="s">
         <v>106</v>
       </c>
@@ -3650,7 +3687,7 @@
       <c r="E19" t="s">
         <v>278</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="13">
         <v>34290</v>
       </c>
       <c r="G19" s="4"/>
@@ -3665,27 +3702,27 @@
       </c>
       <c r="K19" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>76.311441919938275</v>
+        <v>75.141565825502497</v>
       </c>
       <c r="L19" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>80.24794894636949</v>
+        <v>78.268419270573261</v>
       </c>
       <c r="M19" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>79.858519426390416</v>
+        <v>79.833292038267828</v>
       </c>
       <c r="N19" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>43.864731899536153</v>
+        <v>44.696465100568531</v>
       </c>
       <c r="O19" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>69.207236224003879</v>
+        <v>77.647962858182055</v>
       </c>
       <c r="P19" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>87.777281421210375</v>
+        <v>86.289315535861746</v>
       </c>
       <c r="Q19">
         <v>11.5</v>
@@ -3693,8 +3730,8 @@
       <c r="R19" t="s">
         <v>336</v>
       </c>
-      <c r="S19">
-        <v>136</v>
+      <c r="S19" t="s">
+        <v>360</v>
       </c>
       <c r="T19">
         <v>3.4</v>
@@ -3713,42 +3750,42 @@
       </c>
       <c r="Y19" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>32.311441919938275</v>
+        <v>31.141565825502497</v>
       </c>
       <c r="Z19" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>40.24794894636949</v>
+        <v>38.268419270573261</v>
       </c>
       <c r="AA19" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>31.858519426390416</v>
+        <v>31.833292038267828</v>
       </c>
       <c r="AB19" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>25.864731899536153</v>
+        <v>26.696465100568531</v>
       </c>
       <c r="AC19" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>45.670361597718852</v>
+        <v>50.485543251692754</v>
       </c>
       <c r="AD19" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>34.723839786214533</v>
+        <v>34.899390159604039</v>
       </c>
       <c r="AE19" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>12.826471362909901</v>
+        <v>12.578028177035019</v>
       </c>
       <c r="AF19" s="8">
         <v>339</v>
       </c>
-      <c r="AG19" s="8">
+      <c r="AG19" s="8" t="e">
         <f t="shared" ca="1" si="13"/>
-        <v>136.09123814389417</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AH19" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>3.6905118769308918</v>
+        <v>3.644618951821466</v>
       </c>
       <c r="AI19" s="5" t="s">
         <v>224</v>
@@ -3763,7 +3800,7 @@
         <v>53356</v>
       </c>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:38">
       <c r="A20" s="3" t="s">
         <v>107</v>
       </c>
@@ -3779,7 +3816,7 @@
       <c r="E20" t="s">
         <v>278</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="13">
         <v>17590</v>
       </c>
       <c r="G20" s="4"/>
@@ -3794,27 +3831,27 @@
       </c>
       <c r="K20" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>75.518913417132538</v>
+        <v>76.784403687982433</v>
       </c>
       <c r="L20" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>75.391736942664991</v>
+        <v>77.131267106814761</v>
       </c>
       <c r="M20" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>82.122569079480186</v>
+        <v>82.650641893852949</v>
       </c>
       <c r="N20" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>44.398134911379557</v>
+        <v>51.811385434136952</v>
       </c>
       <c r="O20" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>78.610379806709062</v>
+        <v>80.709060996704466</v>
       </c>
       <c r="P20" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>84.109414827344452</v>
+        <v>85.707746124584091</v>
       </c>
       <c r="Q20">
         <v>10.199999999999999</v>
@@ -3822,8 +3859,8 @@
       <c r="R20" t="s">
         <v>328</v>
       </c>
-      <c r="S20">
-        <v>135</v>
+      <c r="S20" t="s">
+        <v>361</v>
       </c>
       <c r="T20">
         <v>3.9</v>
@@ -3842,42 +3879,42 @@
       </c>
       <c r="Y20" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>31.518913417132538</v>
+        <v>32.784403687982433</v>
       </c>
       <c r="Z20" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>35.391736942664991</v>
+        <v>37.131267106814761</v>
       </c>
       <c r="AA20" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>34.122569079480186</v>
+        <v>34.650641893852949</v>
       </c>
       <c r="AB20" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>26.398134911379557</v>
+        <v>33.811385434136952</v>
       </c>
       <c r="AC20" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>52.156857394124785</v>
+        <v>56.455468749139939</v>
       </c>
       <c r="AD20" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>32.54507185333231</v>
+        <v>32.046904204249962</v>
       </c>
       <c r="AE20" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>10.47132832112951</v>
+        <v>10.243360117622775</v>
       </c>
       <c r="AF20" s="8">
         <v>321</v>
       </c>
-      <c r="AG20" s="8">
+      <c r="AG20" s="8" t="e">
         <f t="shared" ca="1" si="13"/>
-        <v>135.42713899777661</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AH20" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>4.0629577364278173</v>
+        <v>3.9652523121028422</v>
       </c>
       <c r="AI20" s="5" t="s">
         <v>227</v>
@@ -3892,7 +3929,7 @@
         <v>32865</v>
       </c>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:38">
       <c r="A21" s="3" t="s">
         <v>108</v>
       </c>
@@ -3908,7 +3945,7 @@
       <c r="E21" t="s">
         <v>279</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="13">
         <v>24219</v>
       </c>
       <c r="G21" s="4"/>
@@ -3923,27 +3960,27 @@
       </c>
       <c r="K21" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>79.013499534638186</v>
+        <v>77.915797294194348</v>
       </c>
       <c r="L21" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>76.122955639340574</v>
+        <v>79.33297175539461</v>
       </c>
       <c r="M21" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>81.587796407465348</v>
+        <v>80.647161775440026</v>
       </c>
       <c r="N21" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>47.75078131941477</v>
+        <v>50.518066209952366</v>
       </c>
       <c r="O21" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>74.589223840313721</v>
+        <v>71.848325505806216</v>
       </c>
       <c r="P21" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>87.665677972566215</v>
+        <v>87.745678547314128</v>
       </c>
       <c r="Q21">
         <v>106</v>
@@ -3951,8 +3988,8 @@
       <c r="R21" t="s">
         <v>337</v>
       </c>
-      <c r="S21">
-        <v>141</v>
+      <c r="S21" t="s">
+        <v>362</v>
       </c>
       <c r="T21">
         <v>4.5999999999999996</v>
@@ -3971,27 +4008,27 @@
       </c>
       <c r="Y21" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>57.013499534638186</v>
+        <v>55.915797294194348</v>
       </c>
       <c r="Z21" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>56.122955639340574</v>
+        <v>59.33297175539461</v>
       </c>
       <c r="AA21" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>57.587796407465348</v>
+        <v>56.647161775440026</v>
       </c>
       <c r="AB21" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>38.75078131941477</v>
+        <v>41.518066209952366</v>
       </c>
       <c r="AC21" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>63.907615387263718</v>
+        <v>60.495800150811107</v>
       </c>
       <c r="AD21" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>62.953150878151966</v>
+        <v>63.032422627810284</v>
       </c>
       <c r="AE21" s="7">
         <v>5.3</v>
@@ -3999,13 +4036,13 @@
       <c r="AF21" s="8">
         <v>349</v>
       </c>
-      <c r="AG21" s="8">
+      <c r="AG21" s="8" t="e">
         <f t="shared" ca="1" si="13"/>
-        <v>141.45694559842849</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AH21" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>4.7160831833592693</v>
+        <v>4.6489819396672445</v>
       </c>
       <c r="AI21" s="5" t="s">
         <v>229</v>
@@ -4020,7 +4057,7 @@
         <v>56772</v>
       </c>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:38">
       <c r="A22" s="3" t="s">
         <v>109</v>
       </c>
@@ -4036,7 +4073,7 @@
       <c r="E22" t="s">
         <v>285</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="13">
         <v>28713</v>
       </c>
       <c r="G22" s="4"/>
@@ -4051,27 +4088,27 @@
       </c>
       <c r="K22" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>51.101468189124944</v>
+        <v>50.387849082820146</v>
       </c>
       <c r="L22" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>54.641160951700307</v>
+        <v>53.018172286378302</v>
       </c>
       <c r="M22" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>54.509647937461729</v>
+        <v>56.122476334359582</v>
       </c>
       <c r="N22" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>33.92322084071472</v>
+        <v>31.578424021558462</v>
       </c>
       <c r="O22" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>49.539685366455409</v>
+        <v>51.582424456172987</v>
       </c>
       <c r="P22" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>58.028191202801601</v>
+        <v>59.070410924074075</v>
       </c>
       <c r="Q22">
         <v>10.1</v>
@@ -4079,8 +4116,8 @@
       <c r="R22" t="s">
         <v>338</v>
       </c>
-      <c r="S22">
-        <v>133</v>
+      <c r="S22" t="s">
+        <v>363</v>
       </c>
       <c r="T22">
         <v>4.3</v>
@@ -4099,19 +4136,19 @@
       </c>
       <c r="Y22" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>7.1014681891249438</v>
+        <v>6.3878490828201464</v>
       </c>
       <c r="Z22" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>14.641160951700307</v>
+        <v>13.018172286378302</v>
       </c>
       <c r="AA22" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>6.5096479374617289</v>
+        <v>8.1224763343595825</v>
       </c>
       <c r="AB22" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>15.92322084071472</v>
+        <v>13.578424021558462</v>
       </c>
       <c r="AC22" s="8" t="s">
         <v>311</v>
@@ -4121,18 +4158,18 @@
       </c>
       <c r="AE22" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>11.272719998762803</v>
+        <v>10.163752904966787</v>
       </c>
       <c r="AF22" s="8">
         <v>216</v>
       </c>
-      <c r="AG22" s="8">
+      <c r="AG22" s="8" t="e">
         <f t="shared" ca="1" si="13"/>
-        <v>133.29857249548121</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AH22" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>4.4475764747643627</v>
+        <v>4.4097848654141973</v>
       </c>
       <c r="AI22" s="5" t="s">
         <v>232</v>
@@ -4147,11 +4184,11 @@
         <v>72594</v>
       </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:38">
       <c r="A23" s="3"/>
       <c r="C23" s="8"/>
       <c r="D23" s="1"/>
-      <c r="F23" s="4"/>
+      <c r="F23" s="13"/>
       <c r="G23" s="4"/>
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
@@ -4174,7 +4211,7 @@
       <c r="AK23" s="5"/>
       <c r="AL23" s="5"/>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:38">
       <c r="A24" s="3" t="s">
         <v>110</v>
       </c>
@@ -4190,7 +4227,7 @@
       <c r="E24" t="s">
         <v>279</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F24" s="13">
         <v>36096</v>
       </c>
       <c r="G24" s="4"/>
@@ -4205,27 +4242,27 @@
       </c>
       <c r="K24" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>76.626453151124721</v>
+        <v>78.457035085402879</v>
       </c>
       <c r="L24" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>76.688999033509774</v>
+        <v>75.029593872930235</v>
       </c>
       <c r="M24" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>78.655405102150127</v>
+        <v>78.691454797988897</v>
       </c>
       <c r="N24" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>50.131789876790094</v>
+        <v>46.207467342302259</v>
       </c>
       <c r="O24" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>75.140580805782676</v>
+        <v>78.03516212705523</v>
       </c>
       <c r="P24" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>87.375416725141051</v>
+        <v>84.677456888914676</v>
       </c>
       <c r="Q24">
         <v>7.3</v>
@@ -4233,8 +4270,8 @@
       <c r="R24" t="s">
         <v>339</v>
       </c>
-      <c r="S24">
-        <v>135</v>
+      <c r="S24" t="s">
+        <v>361</v>
       </c>
       <c r="T24">
         <v>4</v>
@@ -4253,42 +4290,42 @@
       </c>
       <c r="Y24" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>32.626453151124721</v>
+        <v>34.457035085402879</v>
       </c>
       <c r="Z24" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>36.688999033509774</v>
+        <v>35.029593872930235</v>
       </c>
       <c r="AA24" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>30.655405102150127</v>
+        <v>30.691454797988897</v>
       </c>
       <c r="AB24" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>32.131789876790094</v>
+        <v>28.207467342302259</v>
       </c>
       <c r="AC24" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>48.928187168071716</v>
+        <v>51.275274885807043</v>
       </c>
       <c r="AD24" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>33.748962853904921</v>
+        <v>33.022501797020254</v>
       </c>
       <c r="AE24" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>8.197001583564429</v>
+        <v>8.5472020234253865</v>
       </c>
       <c r="AF24" s="8">
         <v>102</v>
       </c>
-      <c r="AG24" s="8">
+      <c r="AG24" s="8" t="e">
         <f t="shared" ca="1" si="13"/>
-        <v>135.32351369469438</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AH24" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>4.2381501590660386</v>
+        <v>4.1190084773109543</v>
       </c>
       <c r="AI24" s="5" t="s">
         <v>235</v>
@@ -4303,7 +4340,7 @@
         <v>29884</v>
       </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:38">
       <c r="A25" s="3" t="s">
         <v>111</v>
       </c>
@@ -4319,7 +4356,7 @@
       <c r="E25" t="s">
         <v>278</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F25" s="13">
         <v>36900</v>
       </c>
       <c r="G25" s="4"/>
@@ -4334,27 +4371,27 @@
       </c>
       <c r="K25" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>78.801900943615095</v>
+        <v>76.459121796355134</v>
       </c>
       <c r="L25" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>75.525340201614469</v>
+        <v>80.723603349104579</v>
       </c>
       <c r="M25" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>82.777689041194122</v>
+        <v>81.752868243610038</v>
       </c>
       <c r="N25" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>44.689985259219057</v>
+        <v>44.269845507283996</v>
       </c>
       <c r="O25" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>80.91448879103055</v>
+        <v>72.502498913579004</v>
       </c>
       <c r="P25" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>84.873464375039845</v>
+        <v>86.303705679798526</v>
       </c>
       <c r="Q25">
         <v>8.6</v>
@@ -4362,8 +4399,8 @@
       <c r="R25" t="s">
         <v>340</v>
       </c>
-      <c r="S25">
-        <v>143</v>
+      <c r="S25" t="s">
+        <v>359</v>
       </c>
       <c r="T25">
         <v>4.0999999999999996</v>
@@ -4382,31 +4419,31 @@
       </c>
       <c r="Y25" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>12.801900943615095</v>
+        <v>10.459121796355134</v>
       </c>
       <c r="Z25" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>15.525340201614469</v>
+        <v>20.723603349104579</v>
       </c>
       <c r="AA25" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>10.777689041194122</v>
+        <v>9.7528682436100382</v>
       </c>
       <c r="AB25" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>17.689985259219057</v>
+        <v>17.269845507283996</v>
       </c>
       <c r="AC25" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>40.210913915767541</v>
+        <v>32.924102029547278</v>
       </c>
       <c r="AD25" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>6.2546895998667447</v>
+        <v>5.7920580759706937</v>
       </c>
       <c r="AE25" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>9.771957772700965</v>
+        <v>9.5696456731932891</v>
       </c>
       <c r="AF25" s="8">
         <v>224</v>
@@ -4430,7 +4467,7 @@
         <v>72529</v>
       </c>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:38">
       <c r="A26" s="3" t="s">
         <v>112</v>
       </c>
@@ -4446,7 +4483,7 @@
       <c r="E26" t="s">
         <v>278</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F26" s="13">
         <v>34400</v>
       </c>
       <c r="G26" s="4"/>
@@ -4461,27 +4498,27 @@
       </c>
       <c r="K26" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>79.155385893372156</v>
+        <v>79.206058971795898</v>
       </c>
       <c r="L26" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>78.400491810118439</v>
+        <v>80.875427328195997</v>
       </c>
       <c r="M26" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>78.430061755480565</v>
+        <v>82.255915895513581</v>
       </c>
       <c r="N26" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>43.764461970432031</v>
+        <v>43.028910847177727</v>
       </c>
       <c r="O26" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>66.242288857140551</v>
+        <v>67.494980887131518</v>
       </c>
       <c r="P26" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>84.185506090314604</v>
+        <v>86.937699455633108</v>
       </c>
       <c r="Q26">
         <v>5.7</v>
@@ -4489,8 +4526,8 @@
       <c r="R26" t="s">
         <v>341</v>
       </c>
-      <c r="S26">
-        <v>136</v>
+      <c r="S26" t="s">
+        <v>360</v>
       </c>
       <c r="T26">
         <v>3.8</v>
@@ -4509,27 +4546,27 @@
       </c>
       <c r="Y26" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>57.155385893372156</v>
+        <v>57.206058971795898</v>
       </c>
       <c r="Z26" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>58.400491810118439</v>
+        <v>60.875427328195997</v>
       </c>
       <c r="AA26" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>54.430061755480565</v>
+        <v>58.255915895513581</v>
       </c>
       <c r="AB26" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>34.764461970432031</v>
+        <v>34.028910847177727</v>
       </c>
       <c r="AC26" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>54.926245098499209</v>
+        <v>56.791138868722925</v>
       </c>
       <c r="AD26" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>59.877478187970048</v>
+        <v>61.760177389133482</v>
       </c>
       <c r="AE26" s="7">
         <v>3.2</v>
@@ -4537,13 +4574,13 @@
       <c r="AF26" s="8">
         <v>242</v>
       </c>
-      <c r="AG26" s="8">
+      <c r="AG26" s="8" t="e">
         <f t="shared" ca="1" si="13"/>
-        <v>136.04885757648489</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AH26" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>3.8816964356092591</v>
+        <v>3.8082053551602635</v>
       </c>
       <c r="AI26" s="5" t="s">
         <v>240</v>
@@ -4558,7 +4595,7 @@
         <v>76681</v>
       </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:38">
       <c r="A27" s="3" t="s">
         <v>113</v>
       </c>
@@ -4574,7 +4611,7 @@
       <c r="E27" t="s">
         <v>278</v>
       </c>
-      <c r="F27" s="4">
+      <c r="F27" s="13">
         <v>31555</v>
       </c>
       <c r="G27" s="4"/>
@@ -4589,27 +4626,27 @@
       </c>
       <c r="K27" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>26.334633697071084</v>
+        <v>25.309765809015346</v>
       </c>
       <c r="L27" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>28.203159403406811</v>
+        <v>28.845202751416203</v>
       </c>
       <c r="M27" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>26.777553989448766</v>
+        <v>28.036813948438926</v>
       </c>
       <c r="N27" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>14.169898748545151</v>
+        <v>19.040327129919461</v>
       </c>
       <c r="O27" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>33.340714186340826</v>
+        <v>22.272986153038481</v>
       </c>
       <c r="P27" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>30.556567776324339</v>
+        <v>29.031427272675472</v>
       </c>
       <c r="Q27">
         <v>9.4</v>
@@ -4617,8 +4654,8 @@
       <c r="R27" t="s">
         <v>342</v>
       </c>
-      <c r="S27">
-        <v>144</v>
+      <c r="S27" t="s">
+        <v>356</v>
       </c>
       <c r="T27">
         <v>3.9</v>
@@ -4637,42 +4674,42 @@
       </c>
       <c r="Y27" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>4.3346336970710837</v>
+        <v>3.3097658090153459</v>
       </c>
       <c r="Z27" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>8.2031594034068114</v>
+        <v>8.8452027514162026</v>
       </c>
       <c r="AA27" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>2.7775539894487657</v>
+        <v>4.036813948438926</v>
       </c>
       <c r="AB27" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>5.1698987485451511</v>
+        <v>10.040327129919461</v>
       </c>
       <c r="AC27" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>22.925691945071755</v>
+        <v>9.2374675682347629</v>
       </c>
       <c r="AD27" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>6.358997858100949</v>
+        <v>4.3085208405025508</v>
       </c>
       <c r="AE27" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>10.302629009130706</v>
+        <v>9.6110647519219441</v>
       </c>
       <c r="AF27" s="8">
         <v>325</v>
       </c>
-      <c r="AG27" s="8">
+      <c r="AG27" s="8" t="e">
         <f t="shared" ca="1" si="13"/>
-        <v>144.4069213728898</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AH27" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>3.9624263303528422</v>
+        <v>3.9053959476838771</v>
       </c>
       <c r="AI27" s="5" t="s">
         <v>243</v>
@@ -4687,7 +4724,7 @@
         <v>98151</v>
       </c>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:38">
       <c r="A28" s="3" t="s">
         <v>114</v>
       </c>
@@ -4703,7 +4740,7 @@
       <c r="E28" t="s">
         <v>279</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F28" s="13">
         <v>21753</v>
       </c>
       <c r="G28" s="4"/>
@@ -4718,27 +4755,27 @@
       </c>
       <c r="K28" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>76.910622361818184</v>
+        <v>79.58982292925937</v>
       </c>
       <c r="L28" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>79.368838047516789</v>
+        <v>76.300662897910613</v>
       </c>
       <c r="M28" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>82.114905007110949</v>
+        <v>80.981879914278565</v>
       </c>
       <c r="N28" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>49.371350207173094</v>
+        <v>50.552197679987515</v>
       </c>
       <c r="O28" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>72.064925430285641</v>
+        <v>73.134858108340822</v>
       </c>
       <c r="P28" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>85.407297229603913</v>
+        <v>84.29993221704548</v>
       </c>
       <c r="Q28">
         <v>8.8000000000000007</v>
@@ -4746,8 +4783,8 @@
       <c r="R28" t="s">
         <v>343</v>
       </c>
-      <c r="S28">
-        <v>145</v>
+      <c r="S28" t="s">
+        <v>357</v>
       </c>
       <c r="T28">
         <v>37</v>
@@ -4766,42 +4803,42 @@
       </c>
       <c r="Y28" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>32.910622361818184</v>
+        <v>35.58982292925937</v>
       </c>
       <c r="Z28" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>39.368838047516789</v>
+        <v>36.300662897910613</v>
       </c>
       <c r="AA28" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>34.114905007110949</v>
+        <v>32.981879914278565</v>
       </c>
       <c r="AB28" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>31.371350207173094</v>
+        <v>32.552197679987515</v>
       </c>
       <c r="AC28" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>45.515319003635092</v>
+        <v>50.048819726242193</v>
       </c>
       <c r="AD28" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>33.105157763943375</v>
+        <v>31.871907371630751</v>
       </c>
       <c r="AE28" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>9.8546820997743385</v>
+        <v>8.9632773803204255</v>
       </c>
       <c r="AF28" s="8">
         <v>356</v>
       </c>
-      <c r="AG28" s="8">
+      <c r="AG28" s="8" t="e">
         <f t="shared" ca="1" si="13"/>
-        <v>145.25745607121334</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AH28" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>37.257296355531459</v>
+        <v>37.096373932907625</v>
       </c>
       <c r="AI28" s="5" t="s">
         <v>245</v>
@@ -4816,7 +4853,7 @@
         <v>33709</v>
       </c>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:38">
       <c r="A29" s="3" t="s">
         <v>115</v>
       </c>
@@ -4832,7 +4869,7 @@
       <c r="E29" t="s">
         <v>283</v>
       </c>
-      <c r="F29" s="4">
+      <c r="F29" s="13">
         <v>33509</v>
       </c>
       <c r="G29" s="4"/>
@@ -4847,27 +4884,27 @@
       </c>
       <c r="K29" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>51.490602169905678</v>
+        <v>51.958720374532355</v>
       </c>
       <c r="L29" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>53.854942268772476</v>
+        <v>54.475567093839793</v>
       </c>
       <c r="M29" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>55.498263848648541</v>
+        <v>56.284175161857959</v>
       </c>
       <c r="N29" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>33.568824863940883</v>
+        <v>36.334543927267205</v>
       </c>
       <c r="O29" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>52.528996913899711</v>
+        <v>56.249228446952209</v>
       </c>
       <c r="P29" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>57.772451419886337</v>
+        <v>58.613561785647406</v>
       </c>
       <c r="Q29">
         <v>5.5</v>
@@ -4875,8 +4912,8 @@
       <c r="R29" t="s">
         <v>163</v>
       </c>
-      <c r="S29">
-        <v>140</v>
+      <c r="S29" t="s">
+        <v>354</v>
       </c>
       <c r="T29">
         <v>4</v>
@@ -4895,27 +4932,27 @@
       </c>
       <c r="Y29" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>29.490602169905678</v>
+        <v>29.958720374532355</v>
       </c>
       <c r="Z29" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>33.854942268772476</v>
+        <v>34.475567093839793</v>
       </c>
       <c r="AA29" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>31.498263848648541</v>
+        <v>32.284175161857959</v>
       </c>
       <c r="AB29" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>24.568824863940883</v>
+        <v>27.334543927267205</v>
       </c>
       <c r="AC29" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>40.148813746051857</v>
+        <v>44.301006303487469</v>
       </c>
       <c r="AD29" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>32.996304133979805</v>
+        <v>33.518274710997069</v>
       </c>
       <c r="AE29" s="7">
         <v>3.3</v>
@@ -4923,13 +4960,13 @@
       <c r="AF29" s="8">
         <v>310</v>
       </c>
-      <c r="AG29" s="8">
+      <c r="AG29" s="8" t="e">
         <f t="shared" ca="1" si="13"/>
-        <v>140.37773478119834</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AH29" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>4.0488942094837457</v>
+        <v>4.2859638941918847</v>
       </c>
       <c r="AI29" s="5" t="s">
         <v>248</v>
@@ -4944,7 +4981,7 @@
         <v>47006</v>
       </c>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:38">
       <c r="A30" s="3" t="s">
         <v>116</v>
       </c>
@@ -4960,7 +4997,7 @@
       <c r="E30" t="s">
         <v>278</v>
       </c>
-      <c r="F30" s="4">
+      <c r="F30" s="13">
         <v>37564</v>
       </c>
       <c r="G30" s="4"/>
@@ -4975,27 +5012,27 @@
       </c>
       <c r="K30" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>77.239374252302198</v>
+        <v>77.673539879300264</v>
       </c>
       <c r="L30" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>80.676455451717231</v>
+        <v>76.635623521852423</v>
       </c>
       <c r="M30" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>81.556714323338113</v>
+        <v>80.034686128763099</v>
       </c>
       <c r="N30" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>44.154595904108234</v>
+        <v>49.119101814009468</v>
       </c>
       <c r="O30" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>73.791784028240912</v>
+        <v>73.825649303304772</v>
       </c>
       <c r="P30" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>84.332748983779425</v>
+        <v>87.717106871567168</v>
       </c>
       <c r="Q30">
         <v>7.6</v>
@@ -5003,8 +5040,8 @@
       <c r="R30" t="s">
         <v>327</v>
       </c>
-      <c r="S30">
-        <v>141</v>
+      <c r="S30" t="s">
+        <v>362</v>
       </c>
       <c r="T30">
         <v>3.6</v>
@@ -5023,42 +5060,42 @@
       </c>
       <c r="Y30" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>11.239374252302198</v>
+        <v>11.673539879300264</v>
       </c>
       <c r="Z30" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>20.676455451717231</v>
+        <v>16.635623521852423</v>
       </c>
       <c r="AA30" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>9.5567143233381131</v>
+        <v>8.0346861287630986</v>
       </c>
       <c r="AB30" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>17.154595904108234</v>
+        <v>22.119101814009468</v>
       </c>
       <c r="AC30" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>32.203811923911005</v>
+        <v>37.396404687299004</v>
       </c>
       <c r="AD30" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>3.8975967497403272</v>
+        <v>8.391476851230367</v>
       </c>
       <c r="AE30" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>8.1516392147727448</v>
+        <v>8.2542194489227327</v>
       </c>
       <c r="AF30" s="8">
         <v>254</v>
       </c>
-      <c r="AG30" s="8">
+      <c r="AG30" s="8" t="e">
         <f t="shared" ca="1" si="13"/>
-        <v>141.17475707938149</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AH30" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>3.8984685096517979</v>
+        <v>3.8659009399538085</v>
       </c>
       <c r="AI30" s="5" t="s">
         <v>250</v>
@@ -5073,7 +5110,7 @@
         <v>55577</v>
       </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:38">
       <c r="A31" s="3" t="s">
         <v>117</v>
       </c>
@@ -5089,7 +5126,7 @@
       <c r="E31" t="s">
         <v>278</v>
       </c>
-      <c r="F31" s="4">
+      <c r="F31" s="13">
         <v>31817</v>
       </c>
       <c r="G31" s="4"/>
@@ -5104,27 +5141,27 @@
       </c>
       <c r="K31" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>75.269749048220859</v>
+        <v>75.3931511577359</v>
       </c>
       <c r="L31" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>75.973781870587743</v>
+        <v>78.11205161309401</v>
       </c>
       <c r="M31" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>80.864622110746083</v>
+        <v>82.02727098708354</v>
       </c>
       <c r="N31" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>49.235788217819355</v>
+        <v>51.583129254891816</v>
       </c>
       <c r="O31" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>67.576340378352981</v>
+        <v>74.034226832339826</v>
       </c>
       <c r="P31" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>84.236443318430091</v>
+        <v>86.922392068386941</v>
       </c>
       <c r="Q31">
         <v>6.3</v>
@@ -5132,8 +5169,8 @@
       <c r="R31" t="s">
         <v>344</v>
       </c>
-      <c r="S31">
-        <v>142</v>
+      <c r="S31" t="s">
+        <v>353</v>
       </c>
       <c r="T31">
         <v>3.5</v>
@@ -5152,27 +5189,27 @@
       </c>
       <c r="Y31" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>53.269749048220859</v>
+        <v>53.3931511577359</v>
       </c>
       <c r="Z31" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>55.973781870587743</v>
+        <v>58.11205161309401</v>
       </c>
       <c r="AA31" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>56.864622110746083</v>
+        <v>58.02727098708354</v>
       </c>
       <c r="AB31" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>40.235788217819355</v>
+        <v>42.583129254891816</v>
       </c>
       <c r="AC31" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>57.813913294452576</v>
+        <v>65.856857349037469</v>
       </c>
       <c r="AD31" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>57.45541648886384</v>
+        <v>60.036289259517105</v>
       </c>
       <c r="AE31" s="7">
         <v>3.7</v>
@@ -5180,13 +5217,13 @@
       <c r="AF31" s="8">
         <v>189</v>
       </c>
-      <c r="AG31" s="8">
+      <c r="AG31" s="8" t="e">
         <f t="shared" ca="1" si="13"/>
-        <v>142.31395784404918</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AH31" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>3.5093779740512892</v>
+        <v>3.6995777047539677</v>
       </c>
       <c r="AI31" s="5" t="s">
         <v>252</v>
@@ -5201,7 +5238,7 @@
         <v>41981</v>
       </c>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:38">
       <c r="A32" s="3" t="s">
         <v>118</v>
       </c>
@@ -5217,7 +5254,7 @@
       <c r="E32" t="s">
         <v>278</v>
       </c>
-      <c r="F32" s="4">
+      <c r="F32" s="13">
         <v>32620</v>
       </c>
       <c r="G32" s="4"/>
@@ -5232,27 +5269,27 @@
       </c>
       <c r="K32" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>76.208090824146396</v>
+        <v>76.97530140658553</v>
       </c>
       <c r="L32" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>78.656897834476894</v>
+        <v>77.103546809564889</v>
       </c>
       <c r="M32" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>82.458677729006041</v>
+        <v>81.437664850761394</v>
       </c>
       <c r="N32" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>47.227931865136767</v>
+        <v>45.086195664000371</v>
       </c>
       <c r="O32" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>74.523945852516547</v>
+        <v>67.776499626693663</v>
       </c>
       <c r="P32" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>84.725128915559921</v>
+        <v>86.07496637284342</v>
       </c>
       <c r="Q32">
         <v>8.9</v>
@@ -5260,8 +5297,8 @@
       <c r="R32" t="s">
         <v>345</v>
       </c>
-      <c r="S32">
-        <v>138</v>
+      <c r="S32" t="s">
+        <v>358</v>
       </c>
       <c r="T32">
         <v>4.5999999999999996</v>
@@ -5280,42 +5317,42 @@
       </c>
       <c r="Y32" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>32.208090824146396</v>
+        <v>32.97530140658553</v>
       </c>
       <c r="Z32" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>38.656897834476894</v>
+        <v>37.103546809564889</v>
       </c>
       <c r="AA32" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>34.458677729006041</v>
+        <v>33.437664850761394</v>
       </c>
       <c r="AB32" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>29.227931865136767</v>
+        <v>27.086195664000371</v>
       </c>
       <c r="AC32" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>48.732521780101422</v>
+        <v>44.006282962193524</v>
       </c>
       <c r="AD32" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>31.614994202397437</v>
+        <v>34.486937949491974</v>
       </c>
       <c r="AE32" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>9.718140963159799</v>
+        <v>9.9469521812470969</v>
       </c>
       <c r="AF32" s="8">
         <v>48</v>
       </c>
-      <c r="AG32" s="8">
+      <c r="AG32" s="8" t="e">
         <f t="shared" ca="1" si="13"/>
-        <v>138.11840912942921</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AH32" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>4.7596721897907859</v>
+        <v>4.6137949504379057</v>
       </c>
       <c r="AI32" s="5" t="s">
         <v>255</v>
@@ -5330,7 +5367,7 @@
         <v>85050</v>
       </c>
     </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:38">
       <c r="A33" s="3" t="s">
         <v>119</v>
       </c>
@@ -5346,7 +5383,7 @@
       <c r="E33" t="s">
         <v>278</v>
       </c>
-      <c r="F33" s="4">
+      <c r="F33" s="13">
         <v>28657</v>
       </c>
       <c r="G33" s="4"/>
@@ -5361,27 +5398,27 @@
       </c>
       <c r="K33" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>75.204703269067295</v>
+        <v>79.409472178117213</v>
       </c>
       <c r="L33" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>75.239449793590509</v>
+        <v>75.483412718846253</v>
       </c>
       <c r="M33" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>78.06552158206965</v>
+        <v>80.591658113807412</v>
       </c>
       <c r="N33" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>47.303543041322982</v>
+        <v>46.624632326326378</v>
       </c>
       <c r="O33" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>80.014468948130641</v>
+        <v>71.164868153292772</v>
       </c>
       <c r="P33" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>84.099620718470945</v>
+        <v>85.776080903291529</v>
       </c>
       <c r="Q33">
         <v>5.9</v>
@@ -5389,8 +5426,8 @@
       <c r="R33" t="s">
         <v>346</v>
       </c>
-      <c r="S33">
-        <v>139</v>
+      <c r="S33" t="s">
+        <v>355</v>
       </c>
       <c r="T33">
         <v>5.0999999999999996</v>
@@ -5409,42 +5446,42 @@
       </c>
       <c r="Y33" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>31.204703269067295</v>
+        <v>35.409472178117213</v>
       </c>
       <c r="Z33" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>35.239449793590509</v>
+        <v>35.483412718846253</v>
       </c>
       <c r="AA33" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>30.06552158206965</v>
+        <v>32.591658113807412</v>
       </c>
       <c r="AB33" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>29.303543041322982</v>
+        <v>28.624632326326378</v>
       </c>
       <c r="AC33" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>56.668132540578398</v>
+        <v>44.753843951114526</v>
       </c>
       <c r="AD33" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>30.144548286446774</v>
+        <v>34.286769402995446</v>
       </c>
       <c r="AE33" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>7.0875471076342462</v>
+        <v>7.1748549196530176</v>
       </c>
       <c r="AF33" s="8">
         <v>1482</v>
       </c>
-      <c r="AG33" s="8">
+      <c r="AG33" s="8" t="e">
         <f t="shared" ca="1" si="13"/>
-        <v>139.27087129938906</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AH33" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>5.3812024580889286</v>
+        <v>5.3710533396868083</v>
       </c>
       <c r="AI33" s="5" t="s">
         <v>258</v>
@@ -5459,7 +5496,7 @@
         <v>41049</v>
       </c>
     </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:38">
       <c r="A34" s="3" t="s">
         <v>120</v>
       </c>
@@ -5475,7 +5512,7 @@
       <c r="E34" t="s">
         <v>318</v>
       </c>
-      <c r="F34" s="4">
+      <c r="F34" s="13">
         <v>31273</v>
       </c>
       <c r="G34" s="4"/>
@@ -5490,27 +5527,27 @@
       </c>
       <c r="K34" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>75.253137452235038</v>
+        <v>79.233420686720777</v>
       </c>
       <c r="L34" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>78.283852189859616</v>
+        <v>76.22939667714968</v>
       </c>
       <c r="M34" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>78.155323782544087</v>
+        <v>80.704509589697579</v>
       </c>
       <c r="N34" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>49.1364227660439</v>
+        <v>47.123986441704488</v>
       </c>
       <c r="O34" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>66.125585114405823</v>
+        <v>76.290691594109276</v>
       </c>
       <c r="P34" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>84.564821646057453</v>
+        <v>86.495762709398321</v>
       </c>
       <c r="Q34">
         <v>6.8</v>
@@ -5518,8 +5555,8 @@
       <c r="R34" t="s">
         <v>347</v>
       </c>
-      <c r="S34">
-        <v>142</v>
+      <c r="S34" t="s">
+        <v>353</v>
       </c>
       <c r="T34" t="s">
         <v>162</v>
@@ -5538,38 +5575,38 @@
       </c>
       <c r="Y34" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>9.2531374522350376</v>
+        <v>13.233420686720777</v>
       </c>
       <c r="Z34" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>18.283852189859616</v>
+        <v>16.22939667714968</v>
       </c>
       <c r="AA34" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>6.1553237825440874</v>
+        <v>8.7045095896975795</v>
       </c>
       <c r="AB34" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>22.1364227660439</v>
+        <v>20.123986441704488</v>
       </c>
       <c r="AC34" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>25.133758473033307</v>
+        <v>37.815308090639157</v>
       </c>
       <c r="AD34" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>4.1646485117858711</v>
+        <v>6.3818766922580545</v>
       </c>
       <c r="AE34" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>7.9728587069581058</v>
+        <v>7.5899161688261261</v>
       </c>
       <c r="AF34" s="8">
         <v>23</v>
       </c>
-      <c r="AG34" s="8">
+      <c r="AG34" s="8" t="e">
         <f t="shared" ca="1" si="13"/>
-        <v>142.31228861661404</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AH34" s="7">
         <v>3.9</v>
@@ -5587,7 +5624,7 @@
         <v>82799</v>
       </c>
     </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:38">
       <c r="A35" s="3" t="s">
         <v>121</v>
       </c>
@@ -5603,7 +5640,7 @@
       <c r="E35" t="s">
         <v>278</v>
       </c>
-      <c r="F35" s="4">
+      <c r="F35" s="13">
         <v>35361</v>
       </c>
       <c r="G35" s="4"/>
@@ -5618,27 +5655,27 @@
       </c>
       <c r="K35" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>53.32482316344624</v>
+        <v>53.27267326976613</v>
       </c>
       <c r="L35" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>53.824002837375886</v>
+        <v>51.32233494113342</v>
       </c>
       <c r="M35" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>53.277662060299235</v>
+        <v>52.452969413767462</v>
       </c>
       <c r="N35" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>31.686004094803693</v>
+        <v>30.548655579408162</v>
       </c>
       <c r="O35" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>54.191133712074709</v>
+        <v>53.784359254888358</v>
       </c>
       <c r="P35" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>58.244335441509243</v>
+        <v>56.126400230658533</v>
       </c>
       <c r="Q35">
         <v>7.8</v>
@@ -5646,8 +5683,8 @@
       <c r="R35" t="s">
         <v>348</v>
       </c>
-      <c r="S35">
-        <v>144</v>
+      <c r="S35" t="s">
+        <v>356</v>
       </c>
       <c r="T35">
         <v>3.6</v>
@@ -5666,27 +5703,27 @@
       </c>
       <c r="Y35" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>31.32482316344624</v>
+        <v>31.27267326976613</v>
       </c>
       <c r="Z35" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>33.824002837375886</v>
+        <v>31.32233494113342</v>
       </c>
       <c r="AA35" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>29.277662060299235</v>
+        <v>28.452969413767462</v>
       </c>
       <c r="AB35" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>22.686004094803693</v>
+        <v>21.548655579408162</v>
       </c>
       <c r="AC35" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>45.492742034115579</v>
+        <v>42.319510025968022</v>
       </c>
       <c r="AD35" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>33.829350704002479</v>
+        <v>31.560941850900136</v>
       </c>
       <c r="AE35" s="7">
         <v>4.5</v>
@@ -5694,13 +5731,13 @@
       <c r="AF35" s="8">
         <v>117</v>
       </c>
-      <c r="AG35" s="8">
+      <c r="AG35" s="8" t="e">
         <f t="shared" ca="1" si="13"/>
-        <v>144.27691515873141</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AH35" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>3.8327385131537275</v>
+        <v>3.865097258961141</v>
       </c>
       <c r="AI35" s="5" t="s">
         <v>263</v>
@@ -5715,7 +5752,7 @@
         <v>72572</v>
       </c>
     </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:38">
       <c r="A36" s="3" t="s">
         <v>122</v>
       </c>
@@ -5731,7 +5768,7 @@
       <c r="E36" t="s">
         <v>278</v>
       </c>
-      <c r="F36" s="4">
+      <c r="F36" s="13">
         <v>28121</v>
       </c>
       <c r="G36" s="4"/>
@@ -5746,27 +5783,27 @@
       </c>
       <c r="K36" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>79.527971739139531</v>
+        <v>75.749252165439387</v>
       </c>
       <c r="L36" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>75.909792862107651</v>
+        <v>75.233100202443694</v>
       </c>
       <c r="M36" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>81.185177927018216</v>
+        <v>78.64488642826764</v>
       </c>
       <c r="N36" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>46.151449044499081</v>
+        <v>43.379516311900005</v>
       </c>
       <c r="O36" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>73.015132515224025</v>
+        <v>76.103140319219762</v>
       </c>
       <c r="P36" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>85.248507882420071</v>
+        <v>85.390476677183187</v>
       </c>
       <c r="Q36">
         <v>6.9</v>
@@ -5774,8 +5811,8 @@
       <c r="R36" t="s">
         <v>349</v>
       </c>
-      <c r="S36">
-        <v>139</v>
+      <c r="S36" t="s">
+        <v>355</v>
       </c>
       <c r="T36">
         <v>4.2</v>
@@ -5794,27 +5831,27 @@
       </c>
       <c r="Y36" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>57.527971739139531</v>
+        <v>53.749252165439387</v>
       </c>
       <c r="Z36" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>55.909792862107651</v>
+        <v>55.233100202443694</v>
       </c>
       <c r="AA36" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>57.185177927018216</v>
+        <v>54.64488642826764</v>
       </c>
       <c r="AB36" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>37.151449044499081</v>
+        <v>34.379516311900005</v>
       </c>
       <c r="AC36" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>60.512142741350772</v>
+        <v>62.836112025007239</v>
       </c>
       <c r="AD36" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>58.881250539203769</v>
+        <v>58.461361176737164</v>
       </c>
       <c r="AE36" s="7">
         <v>4.0999999999999996</v>
@@ -5822,13 +5859,13 @@
       <c r="AF36" s="8">
         <v>381</v>
       </c>
-      <c r="AG36" s="8">
+      <c r="AG36" s="8" t="e">
         <f t="shared" ca="1" si="13"/>
-        <v>139.4747173458656</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AH36" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>4.2925221217198484</v>
+        <v>4.4293486715174373</v>
       </c>
       <c r="AI36" s="5" t="s">
         <v>265</v>
@@ -5843,7 +5880,7 @@
         <v>49770</v>
       </c>
     </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:38">
       <c r="A37" s="3" t="s">
         <v>123</v>
       </c>
@@ -5859,7 +5896,7 @@
       <c r="E37" t="s">
         <v>278</v>
       </c>
-      <c r="F37" s="4">
+      <c r="F37" s="13">
         <v>32157</v>
       </c>
       <c r="G37" s="4"/>
@@ -5874,27 +5911,27 @@
       </c>
       <c r="K37" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>54.56124082310383</v>
+        <v>52.099883008398216</v>
       </c>
       <c r="L37" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>54.872277887949096</v>
+        <v>51.848245847675891</v>
       </c>
       <c r="M37" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>55.045816343866797</v>
+        <v>56.166648294882336</v>
       </c>
       <c r="N37" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>33.204161086171474</v>
+        <v>35.128361123564304</v>
       </c>
       <c r="O37" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>52.939229012828903</v>
+        <v>49.884001932278167</v>
       </c>
       <c r="P37" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>58.843339331423238</v>
+        <v>58.138209572063055</v>
       </c>
       <c r="Q37">
         <v>8.4</v>
@@ -5902,8 +5939,8 @@
       <c r="R37" t="s">
         <v>350</v>
       </c>
-      <c r="S37">
-        <v>138</v>
+      <c r="S37" t="s">
+        <v>358</v>
       </c>
       <c r="T37">
         <v>3.9</v>
@@ -5922,42 +5959,42 @@
       </c>
       <c r="Y37" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>10.56124082310383</v>
+        <v>8.0998830083982156</v>
       </c>
       <c r="Z37" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>14.872277887949096</v>
+        <v>11.848245847675891</v>
       </c>
       <c r="AA37" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>7.0458163438667967</v>
+        <v>8.1666482948823358</v>
       </c>
       <c r="AB37" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>15.204161086171474</v>
+        <v>17.128361123564304</v>
       </c>
       <c r="AC37" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>26.834558419969678</v>
+        <v>22.0336840498199</v>
       </c>
       <c r="AD37" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>7.0183656549231292</v>
+        <v>5.3906854469409167</v>
       </c>
       <c r="AE37" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>9.2101489306060742</v>
+        <v>9.2525029298981245</v>
       </c>
       <c r="AF37" s="8">
         <v>284</v>
       </c>
-      <c r="AG37" s="8">
+      <c r="AG37" s="8" t="e">
         <f t="shared" ca="1" si="13"/>
-        <v>138.41122621835888</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AH37" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>3.9316602227957493</v>
+        <v>3.9539746980283077</v>
       </c>
       <c r="AI37" s="5" t="s">
         <v>272</v>
@@ -5972,7 +6009,7 @@
         <v>34404</v>
       </c>
     </row>
-    <row r="38" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:38">
       <c r="A38" s="3" t="s">
         <v>124</v>
       </c>
@@ -5988,7 +6025,7 @@
       <c r="E38" t="s">
         <v>281</v>
       </c>
-      <c r="F38" s="4">
+      <c r="F38" s="13">
         <v>33361</v>
       </c>
       <c r="G38" s="4"/>
@@ -6003,27 +6040,27 @@
       </c>
       <c r="K38" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>79.455013820399557</v>
+        <v>79.269433716712868</v>
       </c>
       <c r="L38" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>75.790495118248188</v>
+        <v>75.219113746867436</v>
       </c>
       <c r="M38" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>81.425785576603545</v>
+        <v>81.207469009372815</v>
       </c>
       <c r="N38" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>43.89823528149126</v>
+        <v>45.693404543007311</v>
       </c>
       <c r="O38" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>79.983726379083151</v>
+        <v>72.482834195525641</v>
       </c>
       <c r="P38" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>86.602303479596415</v>
+        <v>86.02124495101188</v>
       </c>
       <c r="Q38">
         <v>6.9</v>
@@ -6031,8 +6068,8 @@
       <c r="R38" t="s">
         <v>351</v>
       </c>
-      <c r="S38">
-        <v>140</v>
+      <c r="S38" t="s">
+        <v>354</v>
       </c>
       <c r="T38">
         <v>3.8</v>
@@ -6051,42 +6088,42 @@
       </c>
       <c r="Y38" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>13.455013820399557</v>
+        <v>13.269433716712868</v>
       </c>
       <c r="Z38" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>15.790495118248188</v>
+        <v>15.219113746867436</v>
       </c>
       <c r="AA38" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>9.4257855766035448</v>
+        <v>9.2074690093728151</v>
       </c>
       <c r="AB38" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>16.89823528149126</v>
+        <v>18.693404543007311</v>
       </c>
       <c r="AC38" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>41.96810935780691</v>
+        <v>33.496134073869662</v>
       </c>
       <c r="AD38" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>7.7571497369595352</v>
+        <v>7.9878193381212874</v>
       </c>
       <c r="AE38" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>8.2379325911272971</v>
+        <v>8.0810550242509773</v>
       </c>
       <c r="AF38" s="8">
         <v>229</v>
       </c>
-      <c r="AG38" s="8">
+      <c r="AG38" s="8" t="e">
         <f t="shared" ca="1" si="13"/>
-        <v>140.39017867733247</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AH38" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>3.8629514652306614</v>
+        <v>3.9860435664284046</v>
       </c>
       <c r="AI38" s="5" t="s">
         <v>271</v>
@@ -6104,6 +6141,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6115,18 +6153,18 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="43.5" customWidth="1"/>
     <col min="2" max="2" width="32.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>287</v>
       </c>
@@ -6134,7 +6172,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>290</v>
       </c>
@@ -6142,7 +6180,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>291</v>
       </c>
@@ -6150,7 +6188,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>293</v>
       </c>
@@ -6158,7 +6196,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>294</v>
       </c>
@@ -6166,7 +6204,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>296</v>
       </c>
@@ -6174,7 +6212,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>299</v>
       </c>
@@ -6182,7 +6220,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>303</v>
       </c>
@@ -6190,7 +6228,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>305</v>
       </c>
@@ -6198,7 +6236,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>306</v>
       </c>
@@ -6206,7 +6244,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>308</v>
       </c>
@@ -6214,7 +6252,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>310</v>
       </c>
@@ -6222,7 +6260,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>320</v>
       </c>
@@ -6230,7 +6268,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>322</v>
       </c>

</xml_diff>

<commit_message>
revert dob back to normal date field in excel file
</commit_message>
<xml_diff>
--- a/data/messy_uc.xlsx
+++ b/data/messy_uc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pileggis\Documents\gh-personal\rmedicine-data-cleaning-2023\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30855879-F140-48B5-81ED-D5ED64A04739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAEDC6EA-B47B-4B5B-BC05-C722596B3D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{C3B41A98-E045-B641-B5DC-D433CA053FBE}"/>
   </bookViews>
@@ -1220,7 +1220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1234,7 +1234,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2114,8 +2113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2E3CCE-D9A6-4043-B4E6-790885873B0A}">
   <dimension ref="A1:AL38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
-      <selection activeCell="S32" sqref="S32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2272,7 +2271,7 @@
       <c r="E8" t="s">
         <v>278</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="4">
         <v>38359</v>
       </c>
       <c r="G8" s="4"/>
@@ -2287,27 +2286,27 @@
       </c>
       <c r="K8" s="8">
         <f ca="1">J8*25 + 5* RAND()</f>
-        <v>77.395707089687207</v>
+        <v>75.353380848880235</v>
       </c>
       <c r="L8" s="8">
         <f ca="1">J8* 25 + 6* RAND()</f>
-        <v>75.571492959177732</v>
+        <v>78.881378580334612</v>
       </c>
       <c r="M8" s="8">
         <f ca="1" xml:space="preserve"> J8*26 + 5 * RAND()</f>
-        <v>78.785710925765727</v>
+        <v>79.924644564055058</v>
       </c>
       <c r="N8" s="8">
         <f ca="1" xml:space="preserve"> J8 *14 + 10* RAND()</f>
-        <v>49.664470834109785</v>
+        <v>48.214577300275749</v>
       </c>
       <c r="O8" s="8">
         <f ca="1" xml:space="preserve"> J8 *22 + 15* RAND()</f>
-        <v>76.862692656240355</v>
+        <v>66.9178183661286</v>
       </c>
       <c r="P8" s="8">
         <f ca="1">J8 * 28 + 4* RAND()</f>
-        <v>87.037412004128825</v>
+        <v>87.530944174394577</v>
       </c>
       <c r="Q8">
         <v>8.1999999999999993</v>
@@ -2335,31 +2334,31 @@
       </c>
       <c r="Y8" s="8">
         <f ca="1" xml:space="preserve"> K8-22*(J8-X8)</f>
-        <v>11.395707089687207</v>
+        <v>9.353380848880235</v>
       </c>
       <c r="Z8" s="8">
         <f ca="1" xml:space="preserve"> L8-20*(J8-X8)</f>
-        <v>15.571492959177732</v>
+        <v>18.881378580334612</v>
       </c>
       <c r="AA8" s="8">
         <f ca="1" xml:space="preserve"> M8-24*(J8-X8)</f>
-        <v>6.7857109257657271</v>
+        <v>7.9246445640550576</v>
       </c>
       <c r="AB8" s="8">
         <f ca="1" xml:space="preserve"> N8-9*(J8-X8)</f>
-        <v>22.664470834109785</v>
+        <v>21.214577300275749</v>
       </c>
       <c r="AC8" s="8">
         <f ca="1" xml:space="preserve"> O8-14*(J8-X8)+ 6*RAND()</f>
-        <v>38.794885130798008</v>
+        <v>26.22976077257854</v>
       </c>
       <c r="AD8" s="8">
         <f ca="1" xml:space="preserve"> P8-27*(J8-X8)+ 3*RAND()</f>
-        <v>7.7243079127115006</v>
+        <v>6.6974606598540669</v>
       </c>
       <c r="AE8" s="7">
         <f ca="1">IF(B8 ="upa", Q8 +1.5* RAND()*0.8, Q8 +1.5* RAND())</f>
-        <v>8.5991867886566062</v>
+        <v>9.0222714439999567</v>
       </c>
       <c r="AF8" s="8">
         <v>201</v>
@@ -2370,7 +2369,7 @@
       </c>
       <c r="AH8" s="7">
         <f ca="1">T8 + 0.3* RAND()</f>
-        <v>3.8442296870166284</v>
+        <v>3.9176762538014822</v>
       </c>
       <c r="AI8" s="5" t="s">
         <v>192</v>
@@ -2401,7 +2400,7 @@
       <c r="E9" t="s">
         <v>278</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="4">
         <v>13618</v>
       </c>
       <c r="G9" s="4"/>
@@ -2416,27 +2415,27 @@
       </c>
       <c r="K9" s="8">
         <f t="shared" ref="K9:K38" ca="1" si="0">J9*25 + 5* RAND()</f>
-        <v>52.473553638474939</v>
+        <v>51.845634529023101</v>
       </c>
       <c r="L9" s="8">
         <f t="shared" ref="L9:L38" ca="1" si="1">J9* 25 + 6* RAND()</f>
-        <v>54.111212500317251</v>
+        <v>52.803456190138355</v>
       </c>
       <c r="M9" s="8">
         <f t="shared" ref="M9:M38" ca="1" si="2" xml:space="preserve"> J9*26 + 5 * RAND()</f>
-        <v>53.429761211289502</v>
+        <v>55.751920082900199</v>
       </c>
       <c r="N9" s="8">
         <f t="shared" ref="N9:N38" ca="1" si="3" xml:space="preserve"> J9 *14 + 10* RAND()</f>
-        <v>30.954408451998606</v>
+        <v>35.189819748792615</v>
       </c>
       <c r="O9" s="8">
         <f t="shared" ref="O9:O38" ca="1" si="4" xml:space="preserve"> J9 *22 + 15* RAND()</f>
-        <v>50.728991566923426</v>
+        <v>49.589706426259539</v>
       </c>
       <c r="P9" s="8">
         <f t="shared" ref="P9:P38" ca="1" si="5">J9 * 28 + 4* RAND()</f>
-        <v>56.573732071317323</v>
+        <v>58.860817550868767</v>
       </c>
       <c r="Q9">
         <v>10.1</v>
@@ -2464,31 +2463,31 @@
       </c>
       <c r="Y9" s="8">
         <f t="shared" ref="Y9:Y38" ca="1" si="6" xml:space="preserve"> K9-22*(J9-X9)</f>
-        <v>30.473553638474939</v>
+        <v>29.845634529023101</v>
       </c>
       <c r="Z9" s="8">
         <f t="shared" ref="Z9:Z38" ca="1" si="7" xml:space="preserve"> L9-20*(J9-X9)</f>
-        <v>34.111212500317251</v>
+        <v>32.803456190138355</v>
       </c>
       <c r="AA9" s="8">
         <f t="shared" ref="AA9:AA38" ca="1" si="8" xml:space="preserve"> M9-24*(J9-X9)</f>
-        <v>29.429761211289502</v>
+        <v>31.751920082900199</v>
       </c>
       <c r="AB9" s="8">
         <f t="shared" ref="AB9:AB38" ca="1" si="9" xml:space="preserve"> N9-9*(J9-X9)</f>
-        <v>21.954408451998606</v>
+        <v>26.189819748792615</v>
       </c>
       <c r="AC9" s="8">
         <f t="shared" ref="AC9:AC38" ca="1" si="10" xml:space="preserve"> O9-14*(J9-X9)+ 6*RAND()</f>
-        <v>37.015601200697233</v>
+        <v>39.336355182967225</v>
       </c>
       <c r="AD9" s="8">
         <f t="shared" ref="AD9:AD38" ca="1" si="11" xml:space="preserve"> P9-27*(J9-X9)+ 3*RAND()</f>
-        <v>31.372902794518804</v>
+        <v>34.089470984088095</v>
       </c>
       <c r="AE9" s="7">
         <f t="shared" ref="AE9:AE38" ca="1" si="12">IF(B9 ="upa", Q9 +1.5* RAND()*0.8, Q9 +1.5* RAND())</f>
-        <v>10.644691386643276</v>
+        <v>11.086802118152924</v>
       </c>
       <c r="AF9" s="8">
         <v>340</v>
@@ -2499,7 +2498,7 @@
       </c>
       <c r="AH9" s="7">
         <f t="shared" ref="AH9:AH38" ca="1" si="14">T9 + 0.3* RAND()</f>
-        <v>4.1756809188999311</v>
+        <v>4.2466410585746237</v>
       </c>
       <c r="AI9" s="5" t="s">
         <v>195</v>
@@ -2530,7 +2529,7 @@
       <c r="E10" t="s">
         <v>279</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="4">
         <v>16959</v>
       </c>
       <c r="G10" s="4"/>
@@ -2545,27 +2544,27 @@
       </c>
       <c r="K10" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>28.518112793694499</v>
+        <v>29.005432419381908</v>
       </c>
       <c r="L10" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>27.053633265569317</v>
+        <v>28.087427151826272</v>
       </c>
       <c r="M10" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>30.577025838545786</v>
+        <v>30.012124196427703</v>
       </c>
       <c r="N10" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>14.44579435445258</v>
+        <v>17.960671311566937</v>
       </c>
       <c r="O10" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>28.793691111661211</v>
+        <v>28.50663297441972</v>
       </c>
       <c r="P10" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>31.877770585570026</v>
+        <v>28.014245141812683</v>
       </c>
       <c r="Q10">
         <v>5.5</v>
@@ -2593,27 +2592,27 @@
       </c>
       <c r="Y10" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>28.518112793694499</v>
+        <v>29.005432419381908</v>
       </c>
       <c r="Z10" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>27.053633265569317</v>
+        <v>28.087427151826272</v>
       </c>
       <c r="AA10" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>30.577025838545786</v>
+        <v>30.012124196427703</v>
       </c>
       <c r="AB10" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>14.44579435445258</v>
+        <v>17.960671311566937</v>
       </c>
       <c r="AC10" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>29.336190842822745</v>
+        <v>31.029002950471163</v>
       </c>
       <c r="AD10" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>33.563118436128839</v>
+        <v>28.163906236855443</v>
       </c>
       <c r="AE10" s="7">
         <v>3</v>
@@ -2627,7 +2626,7 @@
       </c>
       <c r="AH10" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>4.4319755120434223</v>
+        <v>4.4776806526215358</v>
       </c>
       <c r="AI10" s="5" t="s">
         <v>198</v>
@@ -2658,7 +2657,7 @@
       <c r="E11" t="s">
         <v>278</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="4">
         <v>23206</v>
       </c>
       <c r="G11" s="4"/>
@@ -2673,27 +2672,27 @@
       </c>
       <c r="K11" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>76.58245982952684</v>
+        <v>76.35963837696319</v>
       </c>
       <c r="L11" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>79.335195839389684</v>
+        <v>78.862061810017536</v>
       </c>
       <c r="M11" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>80.886180167947145</v>
+        <v>82.844771947570862</v>
       </c>
       <c r="N11" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>51.835917542399272</v>
+        <v>51.144819362576172</v>
       </c>
       <c r="O11" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>80.181408383227534</v>
+        <v>77.183154712163983</v>
       </c>
       <c r="P11" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>86.034990715329002</v>
+        <v>87.183874255488661</v>
       </c>
       <c r="Q11">
         <v>4.7</v>
@@ -2721,31 +2720,31 @@
       </c>
       <c r="Y11" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>32.58245982952684</v>
+        <v>32.35963837696319</v>
       </c>
       <c r="Z11" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>39.335195839389684</v>
+        <v>38.862061810017536</v>
       </c>
       <c r="AA11" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>32.886180167947145</v>
+        <v>34.844771947570862</v>
       </c>
       <c r="AB11" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>33.835917542399272</v>
+        <v>33.144819362576172</v>
       </c>
       <c r="AC11" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>55.964249090294992</v>
+        <v>53.220564050596202</v>
       </c>
       <c r="AD11" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>34.716601709177581</v>
+        <v>35.454709639077308</v>
       </c>
       <c r="AE11" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>5.027880204555518</v>
+        <v>4.9775734522474373</v>
       </c>
       <c r="AF11" s="8">
         <v>327</v>
@@ -2756,7 +2755,7 @@
       </c>
       <c r="AH11" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>3.5350948530846789</v>
+        <v>3.5863802171115973</v>
       </c>
       <c r="AI11" s="5" t="s">
         <v>201</v>
@@ -2787,7 +2786,7 @@
       <c r="E12" t="s">
         <v>280</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="4">
         <v>28622</v>
       </c>
       <c r="G12" s="4"/>
@@ -2802,27 +2801,27 @@
       </c>
       <c r="K12" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>77.078132301936236</v>
+        <v>76.334395832019339</v>
       </c>
       <c r="L12" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>77.859580986363056</v>
+        <v>78.09477556283278</v>
       </c>
       <c r="M12" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>80.028365990704103</v>
+        <v>81.234225210717653</v>
       </c>
       <c r="N12" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>43.948922633756297</v>
+        <v>44.650601400773695</v>
       </c>
       <c r="O12" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>71.759208903120197</v>
+        <v>66.089924012239592</v>
       </c>
       <c r="P12" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>87.758663510865873</v>
+        <v>85.215041939119729</v>
       </c>
       <c r="Q12">
         <v>8.9</v>
@@ -2850,27 +2849,27 @@
       </c>
       <c r="Y12" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>55.078132301936236</v>
+        <v>54.334395832019339</v>
       </c>
       <c r="Z12" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>57.859580986363056</v>
+        <v>58.09477556283278</v>
       </c>
       <c r="AA12" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>56.028365990704103</v>
+        <v>57.234225210717653</v>
       </c>
       <c r="AB12" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>34.948922633756297</v>
+        <v>35.650601400773695</v>
       </c>
       <c r="AC12" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>63.018882114525852</v>
+        <v>53.34456349670883</v>
       </c>
       <c r="AD12" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>61.633098344746031</v>
+        <v>60.71780913486478</v>
       </c>
       <c r="AE12" s="7">
         <v>4.8</v>
@@ -2884,7 +2883,7 @@
       </c>
       <c r="AH12" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>4.0714819133176592</v>
+        <v>4.1903698021980116</v>
       </c>
       <c r="AI12" s="5" t="s">
         <v>204</v>
@@ -2915,7 +2914,7 @@
       <c r="E13" t="s">
         <v>281</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="4">
         <v>33697</v>
       </c>
       <c r="G13" s="4"/>
@@ -2930,27 +2929,27 @@
       </c>
       <c r="K13" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>52.690537179484288</v>
+        <v>53.386501302937816</v>
       </c>
       <c r="L13" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>53.932627568006758</v>
+        <v>54.574682326526101</v>
       </c>
       <c r="M13" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>54.306973375632992</v>
+        <v>52.934751994397239</v>
       </c>
       <c r="N13" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>32.735726709985457</v>
+        <v>31.659590258467595</v>
       </c>
       <c r="O13" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>46.837736076125836</v>
+        <v>57.790319955754995</v>
       </c>
       <c r="P13" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>56.276592489518407</v>
+        <v>58.206380126271654</v>
       </c>
       <c r="Q13">
         <v>9.3000000000000007</v>
@@ -2978,31 +2977,31 @@
       </c>
       <c r="Y13" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>30.690537179484288</v>
+        <v>31.386501302937816</v>
       </c>
       <c r="Z13" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>33.932627568006758</v>
+        <v>34.574682326526101</v>
       </c>
       <c r="AA13" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>30.306973375632992</v>
+        <v>28.934751994397239</v>
       </c>
       <c r="AB13" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>23.735726709985457</v>
+        <v>22.659590258467595</v>
       </c>
       <c r="AC13" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>35.823768389183492</v>
+        <v>44.332838097343171</v>
       </c>
       <c r="AD13" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>29.834076609592881</v>
+        <v>32.35099385229492</v>
       </c>
       <c r="AE13" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>9.8411770687840185</v>
+        <v>10.487267983188813</v>
       </c>
       <c r="AF13" s="8">
         <v>348</v>
@@ -3013,7 +3012,7 @@
       </c>
       <c r="AH13" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>4.4564715399867412</v>
+        <v>4.5030140552832183</v>
       </c>
       <c r="AI13" s="5" t="s">
         <v>207</v>
@@ -3044,7 +3043,7 @@
       <c r="E14" t="s">
         <v>282</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="4">
         <v>20323</v>
       </c>
       <c r="G14" s="4"/>
@@ -3059,27 +3058,27 @@
       </c>
       <c r="K14" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>78.029635813522603</v>
+        <v>75.382995948056376</v>
       </c>
       <c r="L14" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>80.314666841608073</v>
+        <v>80.082115996637242</v>
       </c>
       <c r="M14" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>80.405874884577472</v>
+        <v>79.247517849737193</v>
       </c>
       <c r="N14" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>44.450003619478046</v>
+        <v>51.226856036917866</v>
       </c>
       <c r="O14" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>72.174223680967174</v>
+        <v>73.744703401082006</v>
       </c>
       <c r="P14" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>84.869574929335613</v>
+        <v>86.465125336678085</v>
       </c>
       <c r="Q14">
         <v>5.6</v>
@@ -3107,31 +3106,31 @@
       </c>
       <c r="Y14" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>56.029635813522603</v>
+        <v>53.382995948056376</v>
       </c>
       <c r="Z14" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>60.314666841608073</v>
+        <v>60.082115996637242</v>
       </c>
       <c r="AA14" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>56.405874884577472</v>
+        <v>55.247517849737193</v>
       </c>
       <c r="AB14" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>35.450003619478046</v>
+        <v>42.226856036917866</v>
       </c>
       <c r="AC14" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>59.187143457162918</v>
+        <v>65.698843135356029</v>
       </c>
       <c r="AD14" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>60.272050880074822</v>
+        <v>60.911434750452962</v>
       </c>
       <c r="AE14" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>5.8698426976681954</v>
+        <v>6.211863450467038</v>
       </c>
       <c r="AF14" s="8">
         <v>181</v>
@@ -3142,7 +3141,7 @@
       </c>
       <c r="AH14" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>3.8040083057831025</v>
+        <v>3.7121189213199015</v>
       </c>
       <c r="AI14" s="5" t="s">
         <v>210</v>
@@ -3173,7 +3172,7 @@
       <c r="E15" t="s">
         <v>283</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F15" s="4">
         <v>27283</v>
       </c>
       <c r="G15" s="4"/>
@@ -3188,27 +3187,27 @@
       </c>
       <c r="K15" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>79.417740689710314</v>
+        <v>77.502712645960457</v>
       </c>
       <c r="L15" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>78.162622240437145</v>
+        <v>80.330549574087996</v>
       </c>
       <c r="M15" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>82.619855221663997</v>
+        <v>78.069576812980117</v>
       </c>
       <c r="N15" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>45.343555656816527</v>
+        <v>51.569655227287313</v>
       </c>
       <c r="O15" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>80.961274998260961</v>
+        <v>74.591699105959663</v>
       </c>
       <c r="P15" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>84.815926763435428</v>
+        <v>87.629348982318163</v>
       </c>
       <c r="Q15">
         <v>9.6999999999999993</v>
@@ -3236,27 +3235,27 @@
       </c>
       <c r="Y15" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>57.417740689710314</v>
+        <v>55.502712645960457</v>
       </c>
       <c r="Z15" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>58.162622240437145</v>
+        <v>60.330549574087996</v>
       </c>
       <c r="AA15" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>58.619855221663997</v>
+        <v>54.069576812980117</v>
       </c>
       <c r="AB15" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>36.343555656816527</v>
+        <v>42.569655227287313</v>
       </c>
       <c r="AC15" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>70.871157842071199</v>
+        <v>62.804330786921938</v>
       </c>
       <c r="AD15" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>59.517726400153428</v>
+        <v>61.753735844850844</v>
       </c>
       <c r="AE15" s="7">
         <v>4.9000000000000004</v>
@@ -3270,7 +3269,7 @@
       </c>
       <c r="AH15" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>4.6028187814314716</v>
+        <v>4.6739433993045765</v>
       </c>
       <c r="AI15" s="5" t="s">
         <v>213</v>
@@ -3301,7 +3300,7 @@
       <c r="E16" t="s">
         <v>278</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F16" s="4">
         <v>31000</v>
       </c>
       <c r="G16" s="4"/>
@@ -3316,27 +3315,27 @@
       </c>
       <c r="K16" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>50.457859258444074</v>
+        <v>50.804561078752769</v>
       </c>
       <c r="L16" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>52.033617489181125</v>
+        <v>54.522693883565701</v>
       </c>
       <c r="M16" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>54.081207277683689</v>
+        <v>54.448041885969161</v>
       </c>
       <c r="N16" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>37.112809023392508</v>
+        <v>35.277107849750216</v>
       </c>
       <c r="O16" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>57.504151885146584</v>
+        <v>44.369203303817784</v>
       </c>
       <c r="P16" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>57.684203244764717</v>
+        <v>57.275346833851245</v>
       </c>
       <c r="Q16">
         <v>8.3000000000000007</v>
@@ -3364,31 +3363,31 @@
       </c>
       <c r="Y16" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>6.4578592584440742</v>
+        <v>6.8045610787527693</v>
       </c>
       <c r="Z16" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>12.033617489181125</v>
+        <v>14.522693883565701</v>
       </c>
       <c r="AA16" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>6.0812072776836885</v>
+        <v>6.4480418859691611</v>
       </c>
       <c r="AB16" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>19.112809023392508</v>
+        <v>17.277107849750216</v>
       </c>
       <c r="AC16" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>35.271862195951869</v>
+        <v>21.087021696907239</v>
       </c>
       <c r="AD16" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>6.4408767835455043</v>
+        <v>3.5341024329152146</v>
       </c>
       <c r="AE16" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>9.3186188309606344</v>
+        <v>8.5438849647124915</v>
       </c>
       <c r="AF16" s="8">
         <v>135</v>
@@ -3399,7 +3398,7 @@
       </c>
       <c r="AH16" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>4.4311454099701493</v>
+        <v>4.4478713503062721</v>
       </c>
       <c r="AI16" s="5" t="s">
         <v>215</v>
@@ -3430,7 +3429,7 @@
       <c r="E17" t="s">
         <v>278</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="4">
         <v>26653</v>
       </c>
       <c r="G17" s="4"/>
@@ -3445,27 +3444,27 @@
       </c>
       <c r="K17" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>77.374157230637337</v>
+        <v>79.573433483750605</v>
       </c>
       <c r="L17" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>79.766075332759044</v>
+        <v>76.536073311291716</v>
       </c>
       <c r="M17" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>79.074002813637364</v>
+        <v>81.571362469684672</v>
       </c>
       <c r="N17" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>51.10591397561268</v>
+        <v>42.996239346701834</v>
       </c>
       <c r="O17" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>78.540319612546881</v>
+        <v>80.687718540224495</v>
       </c>
       <c r="P17" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>86.051557487358778</v>
+        <v>85.247210711673603</v>
       </c>
       <c r="Q17">
         <v>7.6</v>
@@ -3493,27 +3492,27 @@
       </c>
       <c r="Y17" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>33.374157230637337</v>
+        <v>35.573433483750605</v>
       </c>
       <c r="Z17" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>39.766075332759044</v>
+        <v>36.536073311291716</v>
       </c>
       <c r="AA17" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>31.074002813637364</v>
+        <v>33.571362469684672</v>
       </c>
       <c r="AB17" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>33.10591397561268</v>
+        <v>24.996239346701834</v>
       </c>
       <c r="AC17" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>54.196357092228794</v>
+        <v>57.0852575397004</v>
       </c>
       <c r="AD17" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>33.288576296959846</v>
+        <v>33.609819438433846</v>
       </c>
       <c r="AE17" s="7">
         <v>4.4000000000000004</v>
@@ -3527,7 +3526,7 @@
       </c>
       <c r="AH17" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>3.8766705236733965</v>
+        <v>4.0631416306129786</v>
       </c>
       <c r="AI17" s="5" t="s">
         <v>218</v>
@@ -3558,7 +3557,7 @@
       <c r="E18" t="s">
         <v>284</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="4">
         <v>34617</v>
       </c>
       <c r="G18" s="4"/>
@@ -3573,27 +3572,27 @@
       </c>
       <c r="K18" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>77.447421245422476</v>
+        <v>78.312065895060258</v>
       </c>
       <c r="L18" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>76.098985004396113</v>
+        <v>79.537463682632335</v>
       </c>
       <c r="M18" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>78.770126928081197</v>
+        <v>80.299313969473744</v>
       </c>
       <c r="N18" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>44.676959457398759</v>
+        <v>44.367590059495143</v>
       </c>
       <c r="O18" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>71.055717729270583</v>
+        <v>70.170863328847489</v>
       </c>
       <c r="P18" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>85.214116555222731</v>
+        <v>87.052028328397824</v>
       </c>
       <c r="Q18">
         <v>9.1999999999999993</v>
@@ -3621,31 +3620,31 @@
       </c>
       <c r="Y18" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>11.447421245422476</v>
+        <v>12.312065895060258</v>
       </c>
       <c r="Z18" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>16.098985004396113</v>
+        <v>19.537463682632335</v>
       </c>
       <c r="AA18" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>6.7701269280811971</v>
+        <v>8.2993139694737437</v>
       </c>
       <c r="AB18" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>17.676959457398759</v>
+        <v>17.367590059495143</v>
       </c>
       <c r="AC18" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>32.034063339102154</v>
+        <v>28.859062538961922</v>
       </c>
       <c r="AD18" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>6.9605647288648838</v>
+        <v>7.9424795688286824</v>
       </c>
       <c r="AE18" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>10.017911529361267</v>
+        <v>9.8416690508245441</v>
       </c>
       <c r="AF18" s="8">
         <v>288</v>
@@ -3656,7 +3655,7 @@
       </c>
       <c r="AH18" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>3.6103003129935454</v>
+        <v>3.7225466865155834</v>
       </c>
       <c r="AI18" s="5" t="s">
         <v>221</v>
@@ -3687,7 +3686,7 @@
       <c r="E19" t="s">
         <v>278</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="4">
         <v>34290</v>
       </c>
       <c r="G19" s="4"/>
@@ -3702,27 +3701,27 @@
       </c>
       <c r="K19" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>75.141565825502497</v>
+        <v>75.701060401100264</v>
       </c>
       <c r="L19" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>78.268419270573261</v>
+        <v>80.296890163467978</v>
       </c>
       <c r="M19" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>79.833292038267828</v>
+        <v>82.996641397622383</v>
       </c>
       <c r="N19" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>44.696465100568531</v>
+        <v>46.445273272731413</v>
       </c>
       <c r="O19" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>77.647962858182055</v>
+        <v>66.173268316463165</v>
       </c>
       <c r="P19" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>86.289315535861746</v>
+        <v>84.025569258897633</v>
       </c>
       <c r="Q19">
         <v>11.5</v>
@@ -3750,31 +3749,31 @@
       </c>
       <c r="Y19" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>31.141565825502497</v>
+        <v>31.701060401100264</v>
       </c>
       <c r="Z19" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>38.268419270573261</v>
+        <v>40.296890163467978</v>
       </c>
       <c r="AA19" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>31.833292038267828</v>
+        <v>34.996641397622383</v>
       </c>
       <c r="AB19" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>26.696465100568531</v>
+        <v>28.445273272731413</v>
       </c>
       <c r="AC19" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>50.485543251692754</v>
+        <v>43.693213262803319</v>
       </c>
       <c r="AD19" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>34.899390159604039</v>
+        <v>30.059889683274342</v>
       </c>
       <c r="AE19" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>12.578028177035019</v>
+        <v>11.653817679313516</v>
       </c>
       <c r="AF19" s="8">
         <v>339</v>
@@ -3785,7 +3784,7 @@
       </c>
       <c r="AH19" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>3.644618951821466</v>
+        <v>3.4925428930847642</v>
       </c>
       <c r="AI19" s="5" t="s">
         <v>224</v>
@@ -3816,7 +3815,7 @@
       <c r="E20" t="s">
         <v>278</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F20" s="4">
         <v>17590</v>
       </c>
       <c r="G20" s="4"/>
@@ -3831,27 +3830,27 @@
       </c>
       <c r="K20" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>76.784403687982433</v>
+        <v>75.916414265916728</v>
       </c>
       <c r="L20" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>77.131267106814761</v>
+        <v>79.000570958494919</v>
       </c>
       <c r="M20" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>82.650641893852949</v>
+        <v>79.404214631688049</v>
       </c>
       <c r="N20" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>51.811385434136952</v>
+        <v>51.490875163830644</v>
       </c>
       <c r="O20" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>80.709060996704466</v>
+        <v>78.879706570039758</v>
       </c>
       <c r="P20" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>85.707746124584091</v>
+        <v>85.336184290726621</v>
       </c>
       <c r="Q20">
         <v>10.199999999999999</v>
@@ -3879,31 +3878,31 @@
       </c>
       <c r="Y20" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>32.784403687982433</v>
+        <v>31.916414265916728</v>
       </c>
       <c r="Z20" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>37.131267106814761</v>
+        <v>39.000570958494919</v>
       </c>
       <c r="AA20" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>34.650641893852949</v>
+        <v>31.404214631688049</v>
       </c>
       <c r="AB20" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>33.811385434136952</v>
+        <v>33.490875163830644</v>
       </c>
       <c r="AC20" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>56.455468749139939</v>
+        <v>53.548296507492232</v>
       </c>
       <c r="AD20" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>32.046904204249962</v>
+        <v>31.823897455301598</v>
       </c>
       <c r="AE20" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>10.243360117622775</v>
+        <v>10.531700694352894</v>
       </c>
       <c r="AF20" s="8">
         <v>321</v>
@@ -3914,7 +3913,7 @@
       </c>
       <c r="AH20" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>3.9652523121028422</v>
+        <v>4.1458072809498425</v>
       </c>
       <c r="AI20" s="5" t="s">
         <v>227</v>
@@ -3945,7 +3944,7 @@
       <c r="E21" t="s">
         <v>279</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F21" s="4">
         <v>24219</v>
       </c>
       <c r="G21" s="4"/>
@@ -3960,27 +3959,27 @@
       </c>
       <c r="K21" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>77.915797294194348</v>
+        <v>78.421230015592826</v>
       </c>
       <c r="L21" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>79.33297175539461</v>
+        <v>77.40990751963389</v>
       </c>
       <c r="M21" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>80.647161775440026</v>
+        <v>78.973151329817128</v>
       </c>
       <c r="N21" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>50.518066209952366</v>
+        <v>45.125466586526215</v>
       </c>
       <c r="O21" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>71.848325505806216</v>
+        <v>71.739706630412357</v>
       </c>
       <c r="P21" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>87.745678547314128</v>
+        <v>86.754200308891285</v>
       </c>
       <c r="Q21">
         <v>106</v>
@@ -4008,27 +4007,27 @@
       </c>
       <c r="Y21" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>55.915797294194348</v>
+        <v>56.421230015592826</v>
       </c>
       <c r="Z21" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>59.33297175539461</v>
+        <v>57.40990751963389</v>
       </c>
       <c r="AA21" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>56.647161775440026</v>
+        <v>54.973151329817128</v>
       </c>
       <c r="AB21" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>41.518066209952366</v>
+        <v>36.125466586526215</v>
       </c>
       <c r="AC21" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>60.495800150811107</v>
+        <v>61.209235390962107</v>
       </c>
       <c r="AD21" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>63.032422627810284</v>
+        <v>60.32543371259986</v>
       </c>
       <c r="AE21" s="7">
         <v>5.3</v>
@@ -4042,7 +4041,7 @@
       </c>
       <c r="AH21" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>4.6489819396672445</v>
+        <v>4.7970363039258279</v>
       </c>
       <c r="AI21" s="5" t="s">
         <v>229</v>
@@ -4073,7 +4072,7 @@
       <c r="E22" t="s">
         <v>285</v>
       </c>
-      <c r="F22" s="13">
+      <c r="F22" s="4">
         <v>28713</v>
       </c>
       <c r="G22" s="4"/>
@@ -4088,27 +4087,27 @@
       </c>
       <c r="K22" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>50.387849082820146</v>
+        <v>54.28894969700297</v>
       </c>
       <c r="L22" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>53.018172286378302</v>
+        <v>50.49304153901587</v>
       </c>
       <c r="M22" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>56.122476334359582</v>
+        <v>56.066773727408382</v>
       </c>
       <c r="N22" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>31.578424021558462</v>
+        <v>37.850366217993248</v>
       </c>
       <c r="O22" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>51.582424456172987</v>
+        <v>47.523590636475568</v>
       </c>
       <c r="P22" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>59.070410924074075</v>
+        <v>57.154787476427806</v>
       </c>
       <c r="Q22">
         <v>10.1</v>
@@ -4136,19 +4135,19 @@
       </c>
       <c r="Y22" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>6.3878490828201464</v>
+        <v>10.28894969700297</v>
       </c>
       <c r="Z22" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>13.018172286378302</v>
+        <v>10.49304153901587</v>
       </c>
       <c r="AA22" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>8.1224763343595825</v>
+        <v>8.0667737274083819</v>
       </c>
       <c r="AB22" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>13.578424021558462</v>
+        <v>19.850366217993248</v>
       </c>
       <c r="AC22" s="8" t="s">
         <v>311</v>
@@ -4158,7 +4157,7 @@
       </c>
       <c r="AE22" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>10.163752904966787</v>
+        <v>10.737372640790719</v>
       </c>
       <c r="AF22" s="8">
         <v>216</v>
@@ -4169,7 +4168,7 @@
       </c>
       <c r="AH22" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>4.4097848654141973</v>
+        <v>4.3682980521944197</v>
       </c>
       <c r="AI22" s="5" t="s">
         <v>232</v>
@@ -4188,7 +4187,7 @@
       <c r="A23" s="3"/>
       <c r="C23" s="8"/>
       <c r="D23" s="1"/>
-      <c r="F23" s="13"/>
+      <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
@@ -4227,7 +4226,7 @@
       <c r="E24" t="s">
         <v>279</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F24" s="4">
         <v>36096</v>
       </c>
       <c r="G24" s="4"/>
@@ -4242,27 +4241,27 @@
       </c>
       <c r="K24" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>78.457035085402879</v>
+        <v>79.360849832720291</v>
       </c>
       <c r="L24" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>75.029593872930235</v>
+        <v>78.541761453458122</v>
       </c>
       <c r="M24" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>78.691454797988897</v>
+        <v>81.921000939836986</v>
       </c>
       <c r="N24" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>46.207467342302259</v>
+        <v>43.165396271226555</v>
       </c>
       <c r="O24" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>78.03516212705523</v>
+        <v>74.885707176216911</v>
       </c>
       <c r="P24" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>84.677456888914676</v>
+        <v>87.714831869507194</v>
       </c>
       <c r="Q24">
         <v>7.3</v>
@@ -4290,31 +4289,31 @@
       </c>
       <c r="Y24" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>34.457035085402879</v>
+        <v>35.360849832720291</v>
       </c>
       <c r="Z24" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>35.029593872930235</v>
+        <v>38.541761453458122</v>
       </c>
       <c r="AA24" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>30.691454797988897</v>
+        <v>33.921000939836986</v>
       </c>
       <c r="AB24" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>28.207467342302259</v>
+        <v>25.165396271226555</v>
       </c>
       <c r="AC24" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>51.275274885807043</v>
+        <v>49.500580614048481</v>
       </c>
       <c r="AD24" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>33.022501797020254</v>
+        <v>34.499933305057652</v>
       </c>
       <c r="AE24" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>8.5472020234253865</v>
+        <v>7.4071896849526553</v>
       </c>
       <c r="AF24" s="8">
         <v>102</v>
@@ -4325,7 +4324,7 @@
       </c>
       <c r="AH24" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>4.1190084773109543</v>
+        <v>4.0251941403787859</v>
       </c>
       <c r="AI24" s="5" t="s">
         <v>235</v>
@@ -4356,7 +4355,7 @@
       <c r="E25" t="s">
         <v>278</v>
       </c>
-      <c r="F25" s="13">
+      <c r="F25" s="4">
         <v>36900</v>
       </c>
       <c r="G25" s="4"/>
@@ -4371,27 +4370,27 @@
       </c>
       <c r="K25" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>76.459121796355134</v>
+        <v>77.689157693019382</v>
       </c>
       <c r="L25" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>80.723603349104579</v>
+        <v>76.461605798421488</v>
       </c>
       <c r="M25" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>81.752868243610038</v>
+        <v>79.110692515011948</v>
       </c>
       <c r="N25" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>44.269845507283996</v>
+        <v>45.058949781053336</v>
       </c>
       <c r="O25" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>72.502498913579004</v>
+        <v>69.6035461962272</v>
       </c>
       <c r="P25" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>86.303705679798526</v>
+        <v>85.547361175858256</v>
       </c>
       <c r="Q25">
         <v>8.6</v>
@@ -4419,31 +4418,31 @@
       </c>
       <c r="Y25" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>10.459121796355134</v>
+        <v>11.689157693019382</v>
       </c>
       <c r="Z25" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>20.723603349104579</v>
+        <v>16.461605798421488</v>
       </c>
       <c r="AA25" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>9.7528682436100382</v>
+        <v>7.110692515011948</v>
       </c>
       <c r="AB25" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>17.269845507283996</v>
+        <v>18.058949781053336</v>
       </c>
       <c r="AC25" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>32.924102029547278</v>
+        <v>30.209085604366262</v>
       </c>
       <c r="AD25" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>5.7920580759706937</v>
+        <v>5.1828315316218108</v>
       </c>
       <c r="AE25" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>9.5696456731932891</v>
+        <v>9.0357951474821743</v>
       </c>
       <c r="AF25" s="8">
         <v>224</v>
@@ -4483,7 +4482,7 @@
       <c r="E26" t="s">
         <v>278</v>
       </c>
-      <c r="F26" s="13">
+      <c r="F26" s="4">
         <v>34400</v>
       </c>
       <c r="G26" s="4"/>
@@ -4498,27 +4497,27 @@
       </c>
       <c r="K26" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>79.206058971795898</v>
+        <v>77.965341796764989</v>
       </c>
       <c r="L26" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>80.875427328195997</v>
+        <v>79.606770559442609</v>
       </c>
       <c r="M26" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>82.255915895513581</v>
+        <v>81.923137387453892</v>
       </c>
       <c r="N26" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>43.028910847177727</v>
+        <v>44.87325121133069</v>
       </c>
       <c r="O26" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>67.494980887131518</v>
+        <v>72.967085852819565</v>
       </c>
       <c r="P26" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>86.937699455633108</v>
+        <v>86.942105148185689</v>
       </c>
       <c r="Q26">
         <v>5.7</v>
@@ -4546,27 +4545,27 @@
       </c>
       <c r="Y26" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>57.206058971795898</v>
+        <v>55.965341796764989</v>
       </c>
       <c r="Z26" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>60.875427328195997</v>
+        <v>59.606770559442609</v>
       </c>
       <c r="AA26" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>58.255915895513581</v>
+        <v>57.923137387453892</v>
       </c>
       <c r="AB26" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>34.028910847177727</v>
+        <v>35.87325121133069</v>
       </c>
       <c r="AC26" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>56.791138868722925</v>
+        <v>59.213101229998259</v>
       </c>
       <c r="AD26" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>61.760177389133482</v>
+        <v>62.919277506973444</v>
       </c>
       <c r="AE26" s="7">
         <v>3.2</v>
@@ -4580,7 +4579,7 @@
       </c>
       <c r="AH26" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>3.8082053551602635</v>
+        <v>4.0003497987740291</v>
       </c>
       <c r="AI26" s="5" t="s">
         <v>240</v>
@@ -4611,7 +4610,7 @@
       <c r="E27" t="s">
         <v>278</v>
       </c>
-      <c r="F27" s="13">
+      <c r="F27" s="4">
         <v>31555</v>
       </c>
       <c r="G27" s="4"/>
@@ -4626,27 +4625,27 @@
       </c>
       <c r="K27" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>25.309765809015346</v>
+        <v>29.262812201632727</v>
       </c>
       <c r="L27" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>28.845202751416203</v>
+        <v>30.82478237386157</v>
       </c>
       <c r="M27" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>28.036813948438926</v>
+        <v>29.053565266412402</v>
       </c>
       <c r="N27" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>19.040327129919461</v>
+        <v>14.132393140954232</v>
       </c>
       <c r="O27" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>22.272986153038481</v>
+        <v>35.026076065939527</v>
       </c>
       <c r="P27" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>29.031427272675472</v>
+        <v>30.15340844232875</v>
       </c>
       <c r="Q27">
         <v>9.4</v>
@@ -4674,31 +4673,31 @@
       </c>
       <c r="Y27" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>3.3097658090153459</v>
+        <v>7.2628122016327268</v>
       </c>
       <c r="Z27" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>8.8452027514162026</v>
+        <v>10.82478237386157</v>
       </c>
       <c r="AA27" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>4.036813948438926</v>
+        <v>5.0535652664124022</v>
       </c>
       <c r="AB27" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>10.040327129919461</v>
+        <v>5.1323931409542318</v>
       </c>
       <c r="AC27" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>9.2374675682347629</v>
+        <v>26.112739606372525</v>
       </c>
       <c r="AD27" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>4.3085208405025508</v>
+        <v>3.5112017717662134</v>
       </c>
       <c r="AE27" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>9.6110647519219441</v>
+        <v>10.452011114526611</v>
       </c>
       <c r="AF27" s="8">
         <v>325</v>
@@ -4709,7 +4708,7 @@
       </c>
       <c r="AH27" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>3.9053959476838771</v>
+        <v>3.9370835110742912</v>
       </c>
       <c r="AI27" s="5" t="s">
         <v>243</v>
@@ -4740,7 +4739,7 @@
       <c r="E28" t="s">
         <v>279</v>
       </c>
-      <c r="F28" s="13">
+      <c r="F28" s="4">
         <v>21753</v>
       </c>
       <c r="G28" s="4"/>
@@ -4755,27 +4754,27 @@
       </c>
       <c r="K28" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>79.58982292925937</v>
+        <v>75.482669074827569</v>
       </c>
       <c r="L28" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>76.300662897910613</v>
+        <v>80.86084120787369</v>
       </c>
       <c r="M28" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>80.981879914278565</v>
+        <v>82.120172182404346</v>
       </c>
       <c r="N28" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>50.552197679987515</v>
+        <v>42.723901982567938</v>
       </c>
       <c r="O28" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>73.134858108340822</v>
+        <v>69.115071935928597</v>
       </c>
       <c r="P28" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>84.29993221704548</v>
+        <v>87.52170509974772</v>
       </c>
       <c r="Q28">
         <v>8.8000000000000007</v>
@@ -4803,31 +4802,31 @@
       </c>
       <c r="Y28" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>35.58982292925937</v>
+        <v>31.482669074827569</v>
       </c>
       <c r="Z28" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>36.300662897910613</v>
+        <v>40.86084120787369</v>
       </c>
       <c r="AA28" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>32.981879914278565</v>
+        <v>34.120172182404346</v>
       </c>
       <c r="AB28" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>32.552197679987515</v>
+        <v>24.723901982567938</v>
       </c>
       <c r="AC28" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>50.048819726242193</v>
+        <v>47.007955967492343</v>
       </c>
       <c r="AD28" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>31.871907371630751</v>
+        <v>35.73557407046416</v>
       </c>
       <c r="AE28" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>8.9632773803204255</v>
+        <v>10.126312301371824</v>
       </c>
       <c r="AF28" s="8">
         <v>356</v>
@@ -4838,7 +4837,7 @@
       </c>
       <c r="AH28" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>37.096373932907625</v>
+        <v>37.262219835188866</v>
       </c>
       <c r="AI28" s="5" t="s">
         <v>245</v>
@@ -4869,7 +4868,7 @@
       <c r="E29" t="s">
         <v>283</v>
       </c>
-      <c r="F29" s="13">
+      <c r="F29" s="4">
         <v>33509</v>
       </c>
       <c r="G29" s="4"/>
@@ -4884,27 +4883,27 @@
       </c>
       <c r="K29" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>51.958720374532355</v>
+        <v>54.578968114119959</v>
       </c>
       <c r="L29" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>54.475567093839793</v>
+        <v>51.345063826833126</v>
       </c>
       <c r="M29" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>56.284175161857959</v>
+        <v>55.301663305817712</v>
       </c>
       <c r="N29" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>36.334543927267205</v>
+        <v>35.929863312244095</v>
       </c>
       <c r="O29" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>56.249228446952209</v>
+        <v>52.424164135566684</v>
       </c>
       <c r="P29" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>58.613561785647406</v>
+        <v>58.745249571138835</v>
       </c>
       <c r="Q29">
         <v>5.5</v>
@@ -4932,27 +4931,27 @@
       </c>
       <c r="Y29" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>29.958720374532355</v>
+        <v>32.578968114119959</v>
       </c>
       <c r="Z29" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>34.475567093839793</v>
+        <v>31.345063826833126</v>
       </c>
       <c r="AA29" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>32.284175161857959</v>
+        <v>31.301663305817712</v>
       </c>
       <c r="AB29" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>27.334543927267205</v>
+        <v>26.929863312244095</v>
       </c>
       <c r="AC29" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>44.301006303487469</v>
+        <v>41.125933926707525</v>
       </c>
       <c r="AD29" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>33.518274710997069</v>
+        <v>32.149432993685899</v>
       </c>
       <c r="AE29" s="7">
         <v>3.3</v>
@@ -4966,7 +4965,7 @@
       </c>
       <c r="AH29" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>4.2859638941918847</v>
+        <v>4.0676349325872136</v>
       </c>
       <c r="AI29" s="5" t="s">
         <v>248</v>
@@ -4997,7 +4996,7 @@
       <c r="E30" t="s">
         <v>278</v>
       </c>
-      <c r="F30" s="13">
+      <c r="F30" s="4">
         <v>37564</v>
       </c>
       <c r="G30" s="4"/>
@@ -5012,27 +5011,27 @@
       </c>
       <c r="K30" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>77.673539879300264</v>
+        <v>75.584390544035188</v>
       </c>
       <c r="L30" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>76.635623521852423</v>
+        <v>75.95341586872506</v>
       </c>
       <c r="M30" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>80.034686128763099</v>
+        <v>79.342589989158739</v>
       </c>
       <c r="N30" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>49.119101814009468</v>
+        <v>47.39240423188798</v>
       </c>
       <c r="O30" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>73.825649303304772</v>
+        <v>70.813001097145971</v>
       </c>
       <c r="P30" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>87.717106871567168</v>
+        <v>87.95768419977513</v>
       </c>
       <c r="Q30">
         <v>7.6</v>
@@ -5060,31 +5059,31 @@
       </c>
       <c r="Y30" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>11.673539879300264</v>
+        <v>9.5843905440351875</v>
       </c>
       <c r="Z30" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>16.635623521852423</v>
+        <v>15.95341586872506</v>
       </c>
       <c r="AA30" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>8.0346861287630986</v>
+        <v>7.3425899891587392</v>
       </c>
       <c r="AB30" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>22.119101814009468</v>
+        <v>20.39240423188798</v>
       </c>
       <c r="AC30" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>37.396404687299004</v>
+        <v>29.7334417403755</v>
       </c>
       <c r="AD30" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>8.391476851230367</v>
+        <v>7.90549223338639</v>
       </c>
       <c r="AE30" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>8.2542194489227327</v>
+        <v>7.6013147167676012</v>
       </c>
       <c r="AF30" s="8">
         <v>254</v>
@@ -5095,7 +5094,7 @@
       </c>
       <c r="AH30" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>3.8659009399538085</v>
+        <v>3.8633160202840253</v>
       </c>
       <c r="AI30" s="5" t="s">
         <v>250</v>
@@ -5126,7 +5125,7 @@
       <c r="E31" t="s">
         <v>278</v>
       </c>
-      <c r="F31" s="13">
+      <c r="F31" s="4">
         <v>31817</v>
       </c>
       <c r="G31" s="4"/>
@@ -5141,27 +5140,27 @@
       </c>
       <c r="K31" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>75.3931511577359</v>
+        <v>76.357194095927198</v>
       </c>
       <c r="L31" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>78.11205161309401</v>
+        <v>79.045028665750181</v>
       </c>
       <c r="M31" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>82.02727098708354</v>
+        <v>78.756906794209812</v>
       </c>
       <c r="N31" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>51.583129254891816</v>
+        <v>49.708885741031288</v>
       </c>
       <c r="O31" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>74.034226832339826</v>
+        <v>80.018946115727161</v>
       </c>
       <c r="P31" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>86.922392068386941</v>
+        <v>85.014329262205209</v>
       </c>
       <c r="Q31">
         <v>6.3</v>
@@ -5189,27 +5188,27 @@
       </c>
       <c r="Y31" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>53.3931511577359</v>
+        <v>54.357194095927198</v>
       </c>
       <c r="Z31" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>58.11205161309401</v>
+        <v>59.045028665750181</v>
       </c>
       <c r="AA31" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>58.02727098708354</v>
+        <v>54.756906794209812</v>
       </c>
       <c r="AB31" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>42.583129254891816</v>
+        <v>40.708885741031288</v>
       </c>
       <c r="AC31" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>65.856857349037469</v>
+        <v>67.65406716456701</v>
       </c>
       <c r="AD31" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>60.036289259517105</v>
+        <v>60.80703201736943</v>
       </c>
       <c r="AE31" s="7">
         <v>3.7</v>
@@ -5223,7 +5222,7 @@
       </c>
       <c r="AH31" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>3.6995777047539677</v>
+        <v>3.7776148060683421</v>
       </c>
       <c r="AI31" s="5" t="s">
         <v>252</v>
@@ -5254,7 +5253,7 @@
       <c r="E32" t="s">
         <v>278</v>
       </c>
-      <c r="F32" s="13">
+      <c r="F32" s="4">
         <v>32620</v>
       </c>
       <c r="G32" s="4"/>
@@ -5269,27 +5268,27 @@
       </c>
       <c r="K32" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>76.97530140658553</v>
+        <v>76.814365555863105</v>
       </c>
       <c r="L32" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>77.103546809564889</v>
+        <v>80.224424491939331</v>
       </c>
       <c r="M32" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>81.437664850761394</v>
+        <v>80.746789884233579</v>
       </c>
       <c r="N32" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>45.086195664000371</v>
+        <v>51.719144444045526</v>
       </c>
       <c r="O32" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>67.776499626693663</v>
+        <v>79.626170780918315</v>
       </c>
       <c r="P32" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>86.07496637284342</v>
+        <v>85.619723658910331</v>
       </c>
       <c r="Q32">
         <v>8.9</v>
@@ -5317,31 +5316,31 @@
       </c>
       <c r="Y32" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>32.97530140658553</v>
+        <v>32.814365555863105</v>
       </c>
       <c r="Z32" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>37.103546809564889</v>
+        <v>40.224424491939331</v>
       </c>
       <c r="AA32" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>33.437664850761394</v>
+        <v>32.746789884233579</v>
       </c>
       <c r="AB32" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>27.086195664000371</v>
+        <v>33.719144444045526</v>
       </c>
       <c r="AC32" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>44.006282962193524</v>
+        <v>54.231072540232539</v>
       </c>
       <c r="AD32" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>34.486937949491974</v>
+        <v>33.859159962404391</v>
       </c>
       <c r="AE32" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>9.9469521812470969</v>
+        <v>8.9024061148605078</v>
       </c>
       <c r="AF32" s="8">
         <v>48</v>
@@ -5352,7 +5351,7 @@
       </c>
       <c r="AH32" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>4.6137949504379057</v>
+        <v>4.805851398543834</v>
       </c>
       <c r="AI32" s="5" t="s">
         <v>255</v>
@@ -5383,7 +5382,7 @@
       <c r="E33" t="s">
         <v>278</v>
       </c>
-      <c r="F33" s="13">
+      <c r="F33" s="4">
         <v>28657</v>
       </c>
       <c r="G33" s="4"/>
@@ -5398,27 +5397,27 @@
       </c>
       <c r="K33" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>79.409472178117213</v>
+        <v>78.576171724815637</v>
       </c>
       <c r="L33" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>75.483412718846253</v>
+        <v>80.112628824931363</v>
       </c>
       <c r="M33" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>80.591658113807412</v>
+        <v>80.001786700400004</v>
       </c>
       <c r="N33" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>46.624632326326378</v>
+        <v>48.468180997321717</v>
       </c>
       <c r="O33" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>71.164868153292772</v>
+        <v>66.999873896862312</v>
       </c>
       <c r="P33" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>85.776080903291529</v>
+        <v>87.112025492407625</v>
       </c>
       <c r="Q33">
         <v>5.9</v>
@@ -5446,31 +5445,31 @@
       </c>
       <c r="Y33" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>35.409472178117213</v>
+        <v>34.576171724815637</v>
       </c>
       <c r="Z33" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>35.483412718846253</v>
+        <v>40.112628824931363</v>
       </c>
       <c r="AA33" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>32.591658113807412</v>
+        <v>32.001786700400004</v>
       </c>
       <c r="AB33" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>28.624632326326378</v>
+        <v>30.468180997321717</v>
       </c>
       <c r="AC33" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>44.753843951114526</v>
+        <v>42.399201549145261</v>
       </c>
       <c r="AD33" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>34.286769402995446</v>
+        <v>35.173929505075954</v>
       </c>
       <c r="AE33" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>7.1748549196530176</v>
+        <v>7.1087772168531504</v>
       </c>
       <c r="AF33" s="8">
         <v>1482</v>
@@ -5481,7 +5480,7 @@
       </c>
       <c r="AH33" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>5.3710533396868083</v>
+        <v>5.2589524195947117</v>
       </c>
       <c r="AI33" s="5" t="s">
         <v>258</v>
@@ -5512,7 +5511,7 @@
       <c r="E34" t="s">
         <v>318</v>
       </c>
-      <c r="F34" s="13">
+      <c r="F34" s="4">
         <v>31273</v>
       </c>
       <c r="G34" s="4"/>
@@ -5527,27 +5526,27 @@
       </c>
       <c r="K34" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>79.233420686720777</v>
+        <v>77.085137105693818</v>
       </c>
       <c r="L34" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>76.22939667714968</v>
+        <v>78.00104341864008</v>
       </c>
       <c r="M34" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>80.704509589697579</v>
+        <v>82.90023267477757</v>
       </c>
       <c r="N34" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>47.123986441704488</v>
+        <v>45.143985344765909</v>
       </c>
       <c r="O34" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>76.290691594109276</v>
+        <v>67.991371071914998</v>
       </c>
       <c r="P34" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>86.495762709398321</v>
+        <v>85.244705887004585</v>
       </c>
       <c r="Q34">
         <v>6.8</v>
@@ -5575,31 +5574,31 @@
       </c>
       <c r="Y34" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>13.233420686720777</v>
+        <v>11.085137105693818</v>
       </c>
       <c r="Z34" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>16.22939667714968</v>
+        <v>18.00104341864008</v>
       </c>
       <c r="AA34" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>8.7045095896975795</v>
+        <v>10.90023267477757</v>
       </c>
       <c r="AB34" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>20.123986441704488</v>
+        <v>18.143985344765909</v>
       </c>
       <c r="AC34" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>37.815308090639157</v>
+        <v>26.661585693378196</v>
       </c>
       <c r="AD34" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>6.3818766922580545</v>
+        <v>4.9236333187257619</v>
       </c>
       <c r="AE34" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>7.5899161688261261</v>
+        <v>6.9139185962162877</v>
       </c>
       <c r="AF34" s="8">
         <v>23</v>
@@ -5640,7 +5639,7 @@
       <c r="E35" t="s">
         <v>278</v>
       </c>
-      <c r="F35" s="13">
+      <c r="F35" s="4">
         <v>35361</v>
       </c>
       <c r="G35" s="4"/>
@@ -5655,27 +5654,27 @@
       </c>
       <c r="K35" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>53.27267326976613</v>
+        <v>53.151489401372515</v>
       </c>
       <c r="L35" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>51.32233494113342</v>
+        <v>53.120691801618385</v>
       </c>
       <c r="M35" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>52.452969413767462</v>
+        <v>55.604909329010525</v>
       </c>
       <c r="N35" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>30.548655579408162</v>
+        <v>30.005512243699446</v>
       </c>
       <c r="O35" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>53.784359254888358</v>
+        <v>56.939960008120458</v>
       </c>
       <c r="P35" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>56.126400230658533</v>
+        <v>56.268105392076414</v>
       </c>
       <c r="Q35">
         <v>7.8</v>
@@ -5703,27 +5702,27 @@
       </c>
       <c r="Y35" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>31.27267326976613</v>
+        <v>31.151489401372515</v>
       </c>
       <c r="Z35" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>31.32233494113342</v>
+        <v>33.120691801618385</v>
       </c>
       <c r="AA35" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>28.452969413767462</v>
+        <v>31.604909329010525</v>
       </c>
       <c r="AB35" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>21.548655579408162</v>
+        <v>21.005512243699446</v>
       </c>
       <c r="AC35" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>42.319510025968022</v>
+        <v>43.395734298338397</v>
       </c>
       <c r="AD35" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>31.560941850900136</v>
+        <v>31.29242217625033</v>
       </c>
       <c r="AE35" s="7">
         <v>4.5</v>
@@ -5737,7 +5736,7 @@
       </c>
       <c r="AH35" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>3.865097258961141</v>
+        <v>3.7491189754892642</v>
       </c>
       <c r="AI35" s="5" t="s">
         <v>263</v>
@@ -5768,7 +5767,7 @@
       <c r="E36" t="s">
         <v>278</v>
       </c>
-      <c r="F36" s="13">
+      <c r="F36" s="4">
         <v>28121</v>
       </c>
       <c r="G36" s="4"/>
@@ -5783,27 +5782,27 @@
       </c>
       <c r="K36" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>75.749252165439387</v>
+        <v>77.105587414557704</v>
       </c>
       <c r="L36" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>75.233100202443694</v>
+        <v>77.41323133328396</v>
       </c>
       <c r="M36" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>78.64488642826764</v>
+        <v>79.316747899311594</v>
       </c>
       <c r="N36" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>43.379516311900005</v>
+        <v>46.60178421655575</v>
       </c>
       <c r="O36" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>76.103140319219762</v>
+        <v>76.571818470239549</v>
       </c>
       <c r="P36" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>85.390476677183187</v>
+        <v>86.344686650826105</v>
       </c>
       <c r="Q36">
         <v>6.9</v>
@@ -5831,27 +5830,27 @@
       </c>
       <c r="Y36" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>53.749252165439387</v>
+        <v>55.105587414557704</v>
       </c>
       <c r="Z36" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>55.233100202443694</v>
+        <v>57.41323133328396</v>
       </c>
       <c r="AA36" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>54.64488642826764</v>
+        <v>55.316747899311594</v>
       </c>
       <c r="AB36" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>34.379516311900005</v>
+        <v>37.60178421655575</v>
       </c>
       <c r="AC36" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>62.836112025007239</v>
+        <v>62.852310233019033</v>
       </c>
       <c r="AD36" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>58.461361176737164</v>
+        <v>60.331082838855522</v>
       </c>
       <c r="AE36" s="7">
         <v>4.0999999999999996</v>
@@ -5865,7 +5864,7 @@
       </c>
       <c r="AH36" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>4.4293486715174373</v>
+        <v>4.3539964578798029</v>
       </c>
       <c r="AI36" s="5" t="s">
         <v>265</v>
@@ -5896,7 +5895,7 @@
       <c r="E37" t="s">
         <v>278</v>
       </c>
-      <c r="F37" s="13">
+      <c r="F37" s="4">
         <v>32157</v>
       </c>
       <c r="G37" s="4"/>
@@ -5911,27 +5910,27 @@
       </c>
       <c r="K37" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>52.099883008398216</v>
+        <v>52.329377698341922</v>
       </c>
       <c r="L37" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>51.848245847675891</v>
+        <v>54.936142723277072</v>
       </c>
       <c r="M37" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>56.166648294882336</v>
+        <v>53.780135043424607</v>
       </c>
       <c r="N37" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>35.128361123564304</v>
+        <v>29.542126603735579</v>
       </c>
       <c r="O37" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>49.884001932278167</v>
+        <v>52.495553286232699</v>
       </c>
       <c r="P37" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>58.138209572063055</v>
+        <v>58.456770729394727</v>
       </c>
       <c r="Q37">
         <v>8.4</v>
@@ -5959,31 +5958,31 @@
       </c>
       <c r="Y37" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>8.0998830083982156</v>
+        <v>8.3293776983419221</v>
       </c>
       <c r="Z37" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>11.848245847675891</v>
+        <v>14.936142723277072</v>
       </c>
       <c r="AA37" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>8.1666482948823358</v>
+        <v>5.7801350434246075</v>
       </c>
       <c r="AB37" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>17.128361123564304</v>
+        <v>11.542126603735579</v>
       </c>
       <c r="AC37" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>22.0336840498199</v>
+        <v>27.687965887293004</v>
       </c>
       <c r="AD37" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>5.3906854469409167</v>
+        <v>5.977062493995331</v>
       </c>
       <c r="AE37" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>9.2525029298981245</v>
+        <v>8.9562138181584814</v>
       </c>
       <c r="AF37" s="8">
         <v>284</v>
@@ -5994,7 +5993,7 @@
       </c>
       <c r="AH37" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>3.9539746980283077</v>
+        <v>4.0548308241882545</v>
       </c>
       <c r="AI37" s="5" t="s">
         <v>272</v>
@@ -6025,7 +6024,7 @@
       <c r="E38" t="s">
         <v>281</v>
       </c>
-      <c r="F38" s="13">
+      <c r="F38" s="4">
         <v>33361</v>
       </c>
       <c r="G38" s="4"/>
@@ -6040,27 +6039,27 @@
       </c>
       <c r="K38" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>79.269433716712868</v>
+        <v>78.449598280373138</v>
       </c>
       <c r="L38" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>75.219113746867436</v>
+        <v>77.988616748624764</v>
       </c>
       <c r="M38" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>81.207469009372815</v>
+        <v>78.22780376133872</v>
       </c>
       <c r="N38" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>45.693404543007311</v>
+        <v>45.658489226565045</v>
       </c>
       <c r="O38" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>72.482834195525641</v>
+        <v>69.5612873186153</v>
       </c>
       <c r="P38" s="8">
         <f t="shared" ca="1" si="5"/>
-        <v>86.02124495101188</v>
+        <v>86.443522378207675</v>
       </c>
       <c r="Q38">
         <v>6.9</v>
@@ -6088,31 +6087,31 @@
       </c>
       <c r="Y38" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>13.269433716712868</v>
+        <v>12.449598280373138</v>
       </c>
       <c r="Z38" s="8">
         <f t="shared" ca="1" si="7"/>
-        <v>15.219113746867436</v>
+        <v>17.988616748624764</v>
       </c>
       <c r="AA38" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>9.2074690093728151</v>
+        <v>6.2278037613387198</v>
       </c>
       <c r="AB38" s="8">
         <f t="shared" ca="1" si="9"/>
-        <v>18.693404543007311</v>
+        <v>18.658489226565045</v>
       </c>
       <c r="AC38" s="8">
         <f t="shared" ca="1" si="10"/>
-        <v>33.496134073869662</v>
+        <v>32.200469715310433</v>
       </c>
       <c r="AD38" s="8">
         <f t="shared" ca="1" si="11"/>
-        <v>7.9878193381212874</v>
+        <v>6.1948035746248644</v>
       </c>
       <c r="AE38" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>8.0810550242509773</v>
+        <v>7.4372195157310399</v>
       </c>
       <c r="AF38" s="8">
         <v>229</v>
@@ -6123,7 +6122,7 @@
       </c>
       <c r="AH38" s="7">
         <f t="shared" ca="1" si="14"/>
-        <v>3.9860435664284046</v>
+        <v>3.8864900879415503</v>
       </c>
       <c r="AI38" s="5" t="s">
         <v>271</v>

</xml_diff>